<commit_message>
Update RawPrice without removing NaN
</commit_message>
<xml_diff>
--- a/RawPrice.xlsx
+++ b/RawPrice.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V49"/>
+  <dimension ref="A1:V50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -551,3265 +551,3333 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44228</v>
+        <v>44197</v>
       </c>
       <c r="B2" t="n">
-        <v>13192.35</v>
+        <v>13070.69</v>
       </c>
       <c r="C2" t="n">
-        <v>118.57</v>
+        <v>129.04</v>
       </c>
       <c r="D2" t="n">
-        <v>193.17</v>
+        <v>203.21</v>
       </c>
       <c r="E2" t="n">
-        <v>154.65</v>
+        <v>160.31</v>
       </c>
       <c r="F2" t="n">
-        <v>231.84</v>
+        <v>241.95</v>
       </c>
       <c r="G2" t="n">
-        <v>31.47</v>
+        <v>26.89</v>
       </c>
       <c r="H2" t="n">
-        <v>60.05</v>
+        <v>58.28</v>
       </c>
       <c r="I2" t="n">
-        <v>56.07</v>
+        <v>62.01</v>
       </c>
       <c r="J2" t="n">
-        <v>2</v>
+        <v>1.73</v>
       </c>
       <c r="K2" t="n">
-        <v>141.69</v>
+        <v>145.86</v>
       </c>
       <c r="L2" t="n">
-        <v>132.26</v>
+        <v>114.81</v>
       </c>
       <c r="M2" t="n">
-        <v>10.47</v>
+        <v>11.39</v>
       </c>
       <c r="N2" t="n">
-        <v>35.46</v>
+        <v>31.88</v>
       </c>
       <c r="O2" t="n">
-        <v>15.89</v>
+        <v>15.94</v>
       </c>
       <c r="P2" t="n">
-        <v>445.78</v>
+        <v>504.83</v>
       </c>
       <c r="Q2" t="n">
-        <v>225.17</v>
+        <v>264.51</v>
       </c>
       <c r="R2" t="n">
-        <v>117.37</v>
+        <v>113.25</v>
       </c>
       <c r="S2" t="n">
-        <v>212.55</v>
+        <v>229.08</v>
       </c>
       <c r="T2" t="n">
-        <v>43.5</v>
+        <v>42.61</v>
       </c>
       <c r="U2" t="n">
-        <v>104.02</v>
+        <v>104.43</v>
       </c>
       <c r="V2" t="n">
-        <v>46.07</v>
+        <v>37.99</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44256</v>
+        <v>44228</v>
       </c>
       <c r="B3" t="n">
-        <v>13246.87</v>
+        <v>13192.35</v>
       </c>
       <c r="C3" t="n">
-        <v>119.62</v>
+        <v>118.57</v>
       </c>
       <c r="D3" t="n">
-        <v>213.67</v>
+        <v>193.17</v>
       </c>
       <c r="E3" t="n">
-        <v>154.7</v>
+        <v>154.65</v>
       </c>
       <c r="F3" t="n">
-        <v>255.17</v>
+        <v>231.84</v>
       </c>
       <c r="G3" t="n">
-        <v>35.08</v>
+        <v>31.47</v>
       </c>
       <c r="H3" t="n">
-        <v>65.54000000000001</v>
+        <v>60.05</v>
       </c>
       <c r="I3" t="n">
-        <v>59.69</v>
+        <v>56.07</v>
       </c>
       <c r="J3" t="n">
-        <v>6.48</v>
+        <v>2</v>
       </c>
       <c r="K3" t="n">
-        <v>147.87</v>
+        <v>141.69</v>
       </c>
       <c r="L3" t="n">
-        <v>136.81</v>
+        <v>132.26</v>
       </c>
       <c r="M3" t="n">
-        <v>11.67</v>
+        <v>10.47</v>
       </c>
       <c r="N3" t="n">
-        <v>34.17</v>
+        <v>35.46</v>
       </c>
       <c r="O3" t="n">
-        <v>17.25</v>
+        <v>15.89</v>
       </c>
       <c r="P3" t="n">
-        <v>452.02</v>
+        <v>445.78</v>
       </c>
       <c r="Q3" t="n">
-        <v>222.64</v>
+        <v>225.17</v>
       </c>
       <c r="R3" t="n">
-        <v>110.23</v>
+        <v>117.37</v>
       </c>
       <c r="S3" t="n">
-        <v>214.89</v>
+        <v>212.55</v>
       </c>
       <c r="T3" t="n">
-        <v>45.75</v>
+        <v>43.5</v>
       </c>
       <c r="U3" t="n">
-        <v>121.03</v>
+        <v>104.02</v>
       </c>
       <c r="V3" t="n">
-        <v>48.11</v>
+        <v>46.07</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44287</v>
+        <v>44256</v>
       </c>
       <c r="B4" t="n">
-        <v>13962.68</v>
+        <v>13246.87</v>
       </c>
       <c r="C4" t="n">
-        <v>128.74</v>
+        <v>119.62</v>
       </c>
       <c r="D4" t="n">
-        <v>227.71</v>
+        <v>213.67</v>
       </c>
       <c r="E4" t="n">
-        <v>173.37</v>
+        <v>154.7</v>
       </c>
       <c r="F4" t="n">
-        <v>263.04</v>
+        <v>255.17</v>
       </c>
       <c r="G4" t="n">
-        <v>36.93</v>
+        <v>35.08</v>
       </c>
       <c r="H4" t="n">
-        <v>77.81</v>
+        <v>65.54000000000001</v>
       </c>
       <c r="I4" t="n">
-        <v>56.47</v>
+        <v>59.69</v>
       </c>
       <c r="J4" t="n">
-        <v>7.6</v>
+        <v>6.48</v>
       </c>
       <c r="K4" t="n">
-        <v>146.41</v>
+        <v>147.87</v>
       </c>
       <c r="L4" t="n">
-        <v>138.23</v>
+        <v>136.81</v>
       </c>
       <c r="M4" t="n">
-        <v>11.28</v>
+        <v>11.67</v>
       </c>
       <c r="N4" t="n">
-        <v>33.12</v>
+        <v>34.17</v>
       </c>
       <c r="O4" t="n">
-        <v>17.9</v>
+        <v>17.25</v>
       </c>
       <c r="P4" t="n">
-        <v>466.01</v>
+        <v>452.02</v>
       </c>
       <c r="Q4" t="n">
-        <v>236.48</v>
+        <v>222.64</v>
       </c>
       <c r="R4" t="n">
-        <v>109.21</v>
+        <v>110.23</v>
       </c>
       <c r="S4" t="n">
-        <v>218.2</v>
+        <v>214.89</v>
       </c>
       <c r="T4" t="n">
-        <v>45.46</v>
+        <v>45.75</v>
       </c>
       <c r="U4" t="n">
-        <v>130.04</v>
+        <v>121.03</v>
       </c>
       <c r="V4" t="n">
-        <v>49.32</v>
+        <v>48.11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44317</v>
+        <v>44287</v>
       </c>
       <c r="B5" t="n">
-        <v>13748.74</v>
+        <v>13962.68</v>
       </c>
       <c r="C5" t="n">
-        <v>122.03</v>
+        <v>128.74</v>
       </c>
       <c r="D5" t="n">
-        <v>229.51</v>
+        <v>227.71</v>
       </c>
       <c r="E5" t="n">
-        <v>161.15</v>
+        <v>173.37</v>
       </c>
       <c r="F5" t="n">
-        <v>273.24</v>
+        <v>263.04</v>
       </c>
       <c r="G5" t="n">
-        <v>38.63</v>
+        <v>36.93</v>
       </c>
       <c r="H5" t="n">
-        <v>82.23999999999999</v>
+        <v>77.81</v>
       </c>
       <c r="I5" t="n">
-        <v>61.55</v>
+        <v>56.47</v>
       </c>
       <c r="J5" t="n">
-        <v>8.529999999999999</v>
+        <v>7.6</v>
       </c>
       <c r="K5" t="n">
-        <v>152.28</v>
+        <v>146.41</v>
       </c>
       <c r="L5" t="n">
-        <v>148.47</v>
+        <v>138.23</v>
       </c>
       <c r="M5" t="n">
-        <v>10.1</v>
+        <v>11.28</v>
       </c>
       <c r="N5" t="n">
-        <v>33.65</v>
+        <v>33.12</v>
       </c>
       <c r="O5" t="n">
-        <v>17.15</v>
+        <v>17.9</v>
       </c>
       <c r="P5" t="n">
-        <v>465.28</v>
+        <v>466.01</v>
       </c>
       <c r="Q5" t="n">
-        <v>208.41</v>
+        <v>236.48</v>
       </c>
       <c r="R5" t="n">
-        <v>109.79</v>
+        <v>109.21</v>
       </c>
       <c r="S5" t="n">
-        <v>208.63</v>
+        <v>218.2</v>
       </c>
       <c r="T5" t="n">
-        <v>44.92</v>
+        <v>45.46</v>
       </c>
       <c r="U5" t="n">
-        <v>132.59</v>
+        <v>130.04</v>
       </c>
       <c r="V5" t="n">
-        <v>50.3</v>
+        <v>49.32</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44348</v>
+        <v>44317</v>
       </c>
       <c r="B6" t="n">
-        <v>14503.95</v>
+        <v>13748.74</v>
       </c>
       <c r="C6" t="n">
-        <v>134.35</v>
+        <v>122.03</v>
       </c>
       <c r="D6" t="n">
-        <v>242.7</v>
+        <v>229.51</v>
       </c>
       <c r="E6" t="n">
-        <v>172.01</v>
+        <v>161.15</v>
       </c>
       <c r="F6" t="n">
-        <v>262.31</v>
+        <v>273.24</v>
       </c>
       <c r="G6" t="n">
-        <v>37.57</v>
+        <v>38.63</v>
       </c>
       <c r="H6" t="n">
-        <v>86.20999999999999</v>
+        <v>82.23999999999999</v>
       </c>
       <c r="I6" t="n">
-        <v>58.41</v>
+        <v>61.55</v>
       </c>
       <c r="J6" t="n">
-        <v>7.12</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="K6" t="n">
-        <v>149.14</v>
+        <v>152.28</v>
       </c>
       <c r="L6" t="n">
-        <v>140.6</v>
+        <v>148.47</v>
       </c>
       <c r="M6" t="n">
-        <v>10.13</v>
+        <v>10.1</v>
       </c>
       <c r="N6" t="n">
-        <v>35.52</v>
+        <v>33.65</v>
       </c>
       <c r="O6" t="n">
-        <v>16.77</v>
+        <v>17.15</v>
       </c>
       <c r="P6" t="n">
-        <v>499.94</v>
+        <v>465.28</v>
       </c>
       <c r="Q6" t="n">
-        <v>226.57</v>
+        <v>208.41</v>
       </c>
       <c r="R6" t="n">
-        <v>112.4</v>
+        <v>109.79</v>
       </c>
       <c r="S6" t="n">
-        <v>201.63</v>
+        <v>208.63</v>
       </c>
       <c r="T6" t="n">
-        <v>44.55</v>
+        <v>44.92</v>
       </c>
       <c r="U6" t="n">
-        <v>132.06</v>
+        <v>132.59</v>
       </c>
       <c r="V6" t="n">
-        <v>55.15</v>
+        <v>50.3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44378</v>
+        <v>44348</v>
       </c>
       <c r="B7" t="n">
-        <v>14672.68</v>
+        <v>14503.95</v>
       </c>
       <c r="C7" t="n">
-        <v>143.09</v>
+        <v>134.35</v>
       </c>
       <c r="D7" t="n">
-        <v>255.29</v>
+        <v>242.7</v>
       </c>
       <c r="E7" t="n">
-        <v>166.38</v>
+        <v>172.01</v>
       </c>
       <c r="F7" t="n">
-        <v>266.76</v>
+        <v>262.31</v>
       </c>
       <c r="G7" t="n">
-        <v>35.1</v>
+        <v>37.57</v>
       </c>
       <c r="H7" t="n">
-        <v>102.3</v>
+        <v>86.20999999999999</v>
       </c>
       <c r="I7" t="n">
-        <v>55.41</v>
+        <v>58.41</v>
       </c>
       <c r="J7" t="n">
-        <v>6.6</v>
+        <v>7.12</v>
       </c>
       <c r="K7" t="n">
-        <v>155.9</v>
+        <v>149.14</v>
       </c>
       <c r="L7" t="n">
-        <v>137.21</v>
+        <v>140.6</v>
       </c>
       <c r="M7" t="n">
-        <v>8.76</v>
+        <v>10.13</v>
       </c>
       <c r="N7" t="n">
-        <v>35.71</v>
+        <v>35.52</v>
       </c>
       <c r="O7" t="n">
-        <v>16.35</v>
+        <v>16.77</v>
       </c>
       <c r="P7" t="n">
-        <v>535.46</v>
+        <v>499.94</v>
       </c>
       <c r="Q7" t="n">
-        <v>229.07</v>
+        <v>226.57</v>
       </c>
       <c r="R7" t="n">
-        <v>109.53</v>
+        <v>112.4</v>
       </c>
       <c r="S7" t="n">
-        <v>201.58</v>
+        <v>201.63</v>
       </c>
       <c r="T7" t="n">
-        <v>44.35</v>
+        <v>44.55</v>
       </c>
       <c r="U7" t="n">
-        <v>140.31</v>
+        <v>132.06</v>
       </c>
       <c r="V7" t="n">
-        <v>50.33</v>
+        <v>55.15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44409</v>
+        <v>44378</v>
       </c>
       <c r="B8" t="n">
-        <v>15259.24</v>
+        <v>14672.68</v>
       </c>
       <c r="C8" t="n">
-        <v>148.94</v>
+        <v>143.09</v>
       </c>
       <c r="D8" t="n">
-        <v>263.75</v>
+        <v>255.29</v>
       </c>
       <c r="E8" t="n">
-        <v>173.54</v>
+        <v>166.38</v>
       </c>
       <c r="F8" t="n">
-        <v>247.03</v>
+        <v>266.76</v>
       </c>
       <c r="G8" t="n">
-        <v>38.21</v>
+        <v>35.1</v>
       </c>
       <c r="H8" t="n">
-        <v>112.25</v>
+        <v>102.3</v>
       </c>
       <c r="I8" t="n">
-        <v>55.72</v>
+        <v>55.41</v>
       </c>
       <c r="J8" t="n">
-        <v>6.4</v>
+        <v>6.6</v>
       </c>
       <c r="K8" t="n">
-        <v>156.74</v>
+        <v>155.9</v>
       </c>
       <c r="L8" t="n">
-        <v>145.42</v>
+        <v>137.21</v>
       </c>
       <c r="M8" t="n">
-        <v>9.140000000000001</v>
+        <v>8.76</v>
       </c>
       <c r="N8" t="n">
-        <v>34.96</v>
+        <v>35.71</v>
       </c>
       <c r="O8" t="n">
-        <v>16.37</v>
+        <v>16.35</v>
       </c>
       <c r="P8" t="n">
-        <v>550.27</v>
+        <v>535.46</v>
       </c>
       <c r="Q8" t="n">
-        <v>245.24</v>
+        <v>229.07</v>
       </c>
       <c r="R8" t="n">
-        <v>111.76</v>
+        <v>109.53</v>
       </c>
       <c r="S8" t="n">
-        <v>200.29</v>
+        <v>201.58</v>
       </c>
       <c r="T8" t="n">
-        <v>44.22</v>
+        <v>44.35</v>
       </c>
       <c r="U8" t="n">
-        <v>146.79</v>
+        <v>140.31</v>
       </c>
       <c r="V8" t="n">
-        <v>47.66</v>
+        <v>50.33</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44440</v>
+        <v>44409</v>
       </c>
       <c r="B9" t="n">
-        <v>14448.58</v>
+        <v>15259.24</v>
       </c>
       <c r="C9" t="n">
-        <v>139.02</v>
+        <v>148.94</v>
       </c>
       <c r="D9" t="n">
-        <v>239.59</v>
+        <v>263.75</v>
       </c>
       <c r="E9" t="n">
-        <v>164.25</v>
+        <v>173.54</v>
       </c>
       <c r="F9" t="n">
-        <v>234.75</v>
+        <v>247.03</v>
       </c>
       <c r="G9" t="n">
-        <v>38.85</v>
+        <v>38.21</v>
       </c>
       <c r="H9" t="n">
-        <v>103.87</v>
+        <v>112.25</v>
       </c>
       <c r="I9" t="n">
-        <v>56.76</v>
+        <v>55.72</v>
       </c>
       <c r="J9" t="n">
-        <v>8.199999999999999</v>
+        <v>6.4</v>
       </c>
       <c r="K9" t="n">
-        <v>147.08</v>
+        <v>156.74</v>
       </c>
       <c r="L9" t="n">
-        <v>148.82</v>
+        <v>145.42</v>
       </c>
       <c r="M9" t="n">
-        <v>9.57</v>
+        <v>9.140000000000001</v>
       </c>
       <c r="N9" t="n">
-        <v>39.64</v>
+        <v>34.96</v>
       </c>
       <c r="O9" t="n">
-        <v>16.13</v>
+        <v>16.37</v>
       </c>
       <c r="P9" t="n">
-        <v>566.51</v>
+        <v>550.27</v>
       </c>
       <c r="Q9" t="n">
-        <v>258.49</v>
+        <v>245.24</v>
       </c>
       <c r="R9" t="n">
-        <v>104.84</v>
+        <v>111.76</v>
       </c>
       <c r="S9" t="n">
-        <v>181.39</v>
+        <v>200.29</v>
       </c>
       <c r="T9" t="n">
-        <v>43.43</v>
+        <v>44.22</v>
       </c>
       <c r="U9" t="n">
-        <v>141.35</v>
+        <v>146.79</v>
       </c>
       <c r="V9" t="n">
-        <v>52.2</v>
+        <v>47.66</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44470</v>
+        <v>44440</v>
       </c>
       <c r="B10" t="n">
-        <v>15498.39</v>
+        <v>14448.58</v>
       </c>
       <c r="C10" t="n">
-        <v>147.17</v>
+        <v>139.02</v>
       </c>
       <c r="D10" t="n">
-        <v>255.73</v>
+        <v>239.59</v>
       </c>
       <c r="E10" t="n">
-        <v>168.62</v>
+        <v>164.25</v>
       </c>
       <c r="F10" t="n">
-        <v>276.4</v>
+        <v>234.75</v>
       </c>
       <c r="G10" t="n">
-        <v>43.95</v>
+        <v>38.85</v>
       </c>
       <c r="H10" t="n">
-        <v>123.58</v>
+        <v>103.87</v>
       </c>
       <c r="I10" t="n">
-        <v>59.41</v>
+        <v>56.76</v>
       </c>
       <c r="J10" t="n">
-        <v>10.52</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="K10" t="n">
-        <v>148.34</v>
+        <v>147.08</v>
       </c>
       <c r="L10" t="n">
-        <v>154.46</v>
+        <v>148.82</v>
       </c>
       <c r="M10" t="n">
-        <v>11.56</v>
+        <v>9.57</v>
       </c>
       <c r="N10" t="n">
-        <v>40.84</v>
+        <v>39.64</v>
       </c>
       <c r="O10" t="n">
-        <v>15.08</v>
+        <v>16.13</v>
       </c>
       <c r="P10" t="n">
-        <v>628.03</v>
+        <v>566.51</v>
       </c>
       <c r="Q10" t="n">
-        <v>371.33</v>
+        <v>258.49</v>
       </c>
       <c r="R10" t="n">
-        <v>107.21</v>
+        <v>104.84</v>
       </c>
       <c r="S10" t="n">
-        <v>184.93</v>
+        <v>181.39</v>
       </c>
       <c r="T10" t="n">
-        <v>42.61</v>
+        <v>43.43</v>
       </c>
       <c r="U10" t="n">
-        <v>152.2</v>
+        <v>141.35</v>
       </c>
       <c r="V10" t="n">
-        <v>57.22</v>
+        <v>52.2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44501</v>
+        <v>44470</v>
       </c>
       <c r="B11" t="n">
-        <v>15537.69</v>
+        <v>15498.39</v>
       </c>
       <c r="C11" t="n">
-        <v>162.4</v>
+        <v>147.17</v>
       </c>
       <c r="D11" t="n">
-        <v>238.05</v>
+        <v>255.73</v>
       </c>
       <c r="E11" t="n">
-        <v>175.35</v>
+        <v>168.62</v>
       </c>
       <c r="F11" t="n">
-        <v>264.99</v>
+        <v>276.4</v>
       </c>
       <c r="G11" t="n">
-        <v>40.9</v>
+        <v>43.95</v>
       </c>
       <c r="H11" t="n">
-        <v>127.28</v>
+        <v>123.58</v>
       </c>
       <c r="I11" t="n">
-        <v>58.17</v>
+        <v>59.41</v>
       </c>
       <c r="J11" t="n">
-        <v>14.24</v>
+        <v>10.52</v>
       </c>
       <c r="K11" t="n">
-        <v>142.01</v>
+        <v>148.34</v>
       </c>
       <c r="L11" t="n">
-        <v>145.28</v>
+        <v>154.46</v>
       </c>
       <c r="M11" t="n">
-        <v>11.84</v>
+        <v>11.56</v>
       </c>
       <c r="N11" t="n">
-        <v>37.39</v>
+        <v>40.84</v>
       </c>
       <c r="O11" t="n">
-        <v>13.98</v>
+        <v>15.08</v>
       </c>
       <c r="P11" t="n">
-        <v>627.79</v>
+        <v>628.03</v>
       </c>
       <c r="Q11" t="n">
-        <v>381.59</v>
+        <v>371.33</v>
       </c>
       <c r="R11" t="n">
-        <v>110.46</v>
+        <v>107.21</v>
       </c>
       <c r="S11" t="n">
-        <v>186.94</v>
+        <v>184.93</v>
       </c>
       <c r="T11" t="n">
-        <v>40.9</v>
+        <v>42.61</v>
       </c>
       <c r="U11" t="n">
-        <v>152.62</v>
+        <v>152.2</v>
       </c>
       <c r="V11" t="n">
-        <v>53.11</v>
+        <v>57.22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44531</v>
+        <v>44501</v>
       </c>
       <c r="B12" t="n">
-        <v>15644.97</v>
+        <v>15537.69</v>
       </c>
       <c r="C12" t="n">
-        <v>174.71</v>
+        <v>162.4</v>
       </c>
       <c r="D12" t="n">
-        <v>265.28</v>
+        <v>238.05</v>
       </c>
       <c r="E12" t="n">
-        <v>166.72</v>
+        <v>175.35</v>
       </c>
       <c r="F12" t="n">
-        <v>280.5</v>
+        <v>264.99</v>
       </c>
       <c r="G12" t="n">
-        <v>40.92</v>
+        <v>40.9</v>
       </c>
       <c r="H12" t="n">
-        <v>116.43</v>
+        <v>127.28</v>
       </c>
       <c r="I12" t="n">
-        <v>58.05</v>
+        <v>58.17</v>
       </c>
       <c r="J12" t="n">
-        <v>12.07</v>
+        <v>14.24</v>
       </c>
       <c r="K12" t="n">
-        <v>156.82</v>
+        <v>142.01</v>
       </c>
       <c r="L12" t="n">
-        <v>144.84</v>
+        <v>145.28</v>
       </c>
       <c r="M12" t="n">
-        <v>12.1</v>
+        <v>11.84</v>
       </c>
       <c r="N12" t="n">
-        <v>39.01</v>
+        <v>37.39</v>
       </c>
       <c r="O12" t="n">
-        <v>15.07</v>
+        <v>13.98</v>
       </c>
       <c r="P12" t="n">
-        <v>661.92</v>
+        <v>627.79</v>
       </c>
       <c r="Q12" t="n">
-        <v>352.26</v>
+        <v>381.59</v>
       </c>
       <c r="R12" t="n">
-        <v>113.44</v>
+        <v>110.46</v>
       </c>
       <c r="S12" t="n">
-        <v>219.6</v>
+        <v>186.94</v>
       </c>
       <c r="T12" t="n">
-        <v>42.28</v>
+        <v>40.9</v>
       </c>
       <c r="U12" t="n">
-        <v>158.54</v>
+        <v>152.62</v>
       </c>
       <c r="V12" t="n">
-        <v>55.03</v>
+        <v>53.11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44562</v>
+        <v>44531</v>
       </c>
       <c r="B13" t="n">
-        <v>14239.88</v>
+        <v>15644.97</v>
       </c>
       <c r="C13" t="n">
-        <v>171.96</v>
+        <v>174.71</v>
       </c>
       <c r="D13" t="n">
-        <v>229.23</v>
+        <v>265.28</v>
       </c>
       <c r="E13" t="n">
-        <v>149.57</v>
+        <v>166.72</v>
       </c>
       <c r="F13" t="n">
-        <v>261.38</v>
+        <v>280.5</v>
       </c>
       <c r="G13" t="n">
-        <v>42.64</v>
+        <v>40.92</v>
       </c>
       <c r="H13" t="n">
-        <v>118.75</v>
+        <v>116.43</v>
       </c>
       <c r="I13" t="n">
-        <v>57.63</v>
+        <v>58.05</v>
       </c>
       <c r="J13" t="n">
-        <v>11.6</v>
+        <v>12.07</v>
       </c>
       <c r="K13" t="n">
-        <v>157.93</v>
+        <v>156.82</v>
       </c>
       <c r="L13" t="n">
-        <v>135.92</v>
+        <v>144.84</v>
       </c>
       <c r="M13" t="n">
-        <v>12.75</v>
+        <v>12.1</v>
       </c>
       <c r="N13" t="n">
-        <v>46.19</v>
+        <v>39.01</v>
       </c>
       <c r="O13" t="n">
-        <v>15.62</v>
+        <v>15.07</v>
       </c>
       <c r="P13" t="n">
-        <v>576.9</v>
+        <v>661.92</v>
       </c>
       <c r="Q13" t="n">
-        <v>312.24</v>
+        <v>352.26</v>
       </c>
       <c r="R13" t="n">
-        <v>116.11</v>
+        <v>113.44</v>
       </c>
       <c r="S13" t="n">
-        <v>243.05</v>
+        <v>219.6</v>
       </c>
       <c r="T13" t="n">
-        <v>43.31</v>
+        <v>42.28</v>
       </c>
       <c r="U13" t="n">
-        <v>143.42</v>
+        <v>158.54</v>
       </c>
       <c r="V13" t="n">
-        <v>68.31999999999999</v>
+        <v>55.03</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44593</v>
+        <v>44562</v>
       </c>
       <c r="B14" t="n">
-        <v>13751.4</v>
+        <v>14239.88</v>
       </c>
       <c r="C14" t="n">
-        <v>162.46</v>
+        <v>171.96</v>
       </c>
       <c r="D14" t="n">
-        <v>206.78</v>
+        <v>229.23</v>
       </c>
       <c r="E14" t="n">
-        <v>153.56</v>
+        <v>149.57</v>
       </c>
       <c r="F14" t="n">
-        <v>218.93</v>
+        <v>261.38</v>
       </c>
       <c r="G14" t="n">
-        <v>40.85</v>
+        <v>42.64</v>
       </c>
       <c r="H14" t="n">
-        <v>114.7</v>
+        <v>118.75</v>
       </c>
       <c r="I14" t="n">
-        <v>58.01</v>
+        <v>57.63</v>
       </c>
       <c r="J14" t="n">
-        <v>11.8</v>
+        <v>11.6</v>
       </c>
       <c r="K14" t="n">
-        <v>150.86</v>
+        <v>157.93</v>
       </c>
       <c r="L14" t="n">
-        <v>130.48</v>
+        <v>135.92</v>
       </c>
       <c r="M14" t="n">
-        <v>11.33</v>
+        <v>12.75</v>
       </c>
       <c r="N14" t="n">
-        <v>47.08</v>
+        <v>46.19</v>
       </c>
       <c r="O14" t="n">
-        <v>14.9</v>
+        <v>15.62</v>
       </c>
       <c r="P14" t="n">
-        <v>539.88</v>
+        <v>576.9</v>
       </c>
       <c r="Q14" t="n">
-        <v>290.14</v>
+        <v>312.24</v>
       </c>
       <c r="R14" t="n">
-        <v>101.32</v>
+        <v>116.11</v>
       </c>
       <c r="S14" t="n">
-        <v>230.02</v>
+        <v>243.05</v>
       </c>
       <c r="T14" t="n">
-        <v>44.19</v>
+        <v>43.31</v>
       </c>
       <c r="U14" t="n">
-        <v>137.66</v>
+        <v>143.42</v>
       </c>
       <c r="V14" t="n">
-        <v>70.53</v>
+        <v>68.31999999999999</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44621</v>
+        <v>44593</v>
       </c>
       <c r="B15" t="n">
-        <v>14220.52</v>
+        <v>13751.4</v>
       </c>
       <c r="C15" t="n">
-        <v>172.01</v>
+        <v>162.46</v>
       </c>
       <c r="D15" t="n">
-        <v>228.97</v>
+        <v>206.78</v>
       </c>
       <c r="E15" t="n">
-        <v>163</v>
+        <v>153.56</v>
       </c>
       <c r="F15" t="n">
-        <v>231.54</v>
+        <v>218.93</v>
       </c>
       <c r="G15" t="n">
-        <v>38.1</v>
+        <v>40.85</v>
       </c>
       <c r="H15" t="n">
-        <v>115.47</v>
+        <v>114.7</v>
       </c>
       <c r="I15" t="n">
-        <v>56.08</v>
+        <v>58.01</v>
       </c>
       <c r="J15" t="n">
-        <v>18.79</v>
+        <v>11.8</v>
       </c>
       <c r="K15" t="n">
-        <v>163.51</v>
+        <v>150.86</v>
       </c>
       <c r="L15" t="n">
-        <v>125.43</v>
+        <v>130.48</v>
       </c>
       <c r="M15" t="n">
-        <v>11.9</v>
+        <v>11.33</v>
       </c>
       <c r="N15" t="n">
-        <v>49.37</v>
+        <v>47.08</v>
       </c>
       <c r="O15" t="n">
-        <v>14.86</v>
+        <v>14.9</v>
       </c>
       <c r="P15" t="n">
-        <v>586.1799999999999</v>
+        <v>539.88</v>
       </c>
       <c r="Q15" t="n">
-        <v>359.2</v>
+        <v>290.14</v>
       </c>
       <c r="R15" t="n">
-        <v>98.70999999999999</v>
+        <v>101.32</v>
       </c>
       <c r="S15" t="n">
-        <v>260.97</v>
+        <v>230.02</v>
       </c>
       <c r="T15" t="n">
-        <v>41.95</v>
+        <v>44.19</v>
       </c>
       <c r="U15" t="n">
-        <v>151.1</v>
+        <v>137.66</v>
       </c>
       <c r="V15" t="n">
-        <v>75.11</v>
+        <v>70.53</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44652</v>
+        <v>44621</v>
       </c>
       <c r="B16" t="n">
-        <v>12334.64</v>
+        <v>14220.52</v>
       </c>
       <c r="C16" t="n">
-        <v>155.31</v>
+        <v>172.01</v>
       </c>
       <c r="D16" t="n">
-        <v>219.67</v>
+        <v>228.97</v>
       </c>
       <c r="E16" t="n">
-        <v>124.28</v>
+        <v>163</v>
       </c>
       <c r="F16" t="n">
-        <v>218.26</v>
+        <v>231.54</v>
       </c>
       <c r="G16" t="n">
-        <v>33.14</v>
+        <v>38.1</v>
       </c>
       <c r="H16" t="n">
-        <v>92.40000000000001</v>
+        <v>115.47</v>
       </c>
       <c r="I16" t="n">
-        <v>56.52</v>
+        <v>56.08</v>
       </c>
       <c r="J16" t="n">
-        <v>23.8</v>
+        <v>18.79</v>
       </c>
       <c r="K16" t="n">
-        <v>166.49</v>
+        <v>163.51</v>
       </c>
       <c r="L16" t="n">
-        <v>109.83</v>
+        <v>125.43</v>
       </c>
       <c r="M16" t="n">
-        <v>12.61</v>
+        <v>11.9</v>
       </c>
       <c r="N16" t="n">
-        <v>48.02</v>
+        <v>49.37</v>
       </c>
       <c r="O16" t="n">
-        <v>15.71</v>
+        <v>14.86</v>
       </c>
       <c r="P16" t="n">
-        <v>549.04</v>
+        <v>586.1799999999999</v>
       </c>
       <c r="Q16" t="n">
-        <v>290.25</v>
+        <v>359.2</v>
       </c>
       <c r="R16" t="n">
-        <v>88.41</v>
+        <v>98.70999999999999</v>
       </c>
       <c r="S16" t="n">
-        <v>273.22</v>
+        <v>260.97</v>
       </c>
       <c r="T16" t="n">
-        <v>38.13</v>
+        <v>41.95</v>
       </c>
       <c r="U16" t="n">
-        <v>157.42</v>
+        <v>151.1</v>
       </c>
       <c r="V16" t="n">
-        <v>77.52</v>
+        <v>75.11</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44682</v>
+        <v>44652</v>
       </c>
       <c r="B17" t="n">
-        <v>12081.39</v>
+        <v>12334.64</v>
       </c>
       <c r="C17" t="n">
-        <v>146.63</v>
+        <v>155.31</v>
       </c>
       <c r="D17" t="n">
-        <v>234.69</v>
+        <v>219.67</v>
       </c>
       <c r="E17" t="n">
-        <v>120.21</v>
+        <v>124.28</v>
       </c>
       <c r="F17" t="n">
-        <v>229.53</v>
+        <v>218.26</v>
       </c>
       <c r="G17" t="n">
-        <v>34.55</v>
+        <v>33.14</v>
       </c>
       <c r="H17" t="n">
-        <v>108.47</v>
+        <v>92.40000000000001</v>
       </c>
       <c r="I17" t="n">
-        <v>57.85</v>
+        <v>56.52</v>
       </c>
       <c r="J17" t="n">
-        <v>20.98</v>
+        <v>23.8</v>
       </c>
       <c r="K17" t="n">
-        <v>165.63</v>
+        <v>166.49</v>
       </c>
       <c r="L17" t="n">
-        <v>122.57</v>
+        <v>109.83</v>
       </c>
       <c r="M17" t="n">
-        <v>12.16</v>
+        <v>12.61</v>
       </c>
       <c r="N17" t="n">
-        <v>53.22</v>
+        <v>48.02</v>
       </c>
       <c r="O17" t="n">
-        <v>17.99</v>
+        <v>15.71</v>
       </c>
       <c r="P17" t="n">
-        <v>563.59</v>
+        <v>549.04</v>
       </c>
       <c r="Q17" t="n">
-        <v>252.75</v>
+        <v>290.25</v>
       </c>
       <c r="R17" t="n">
-        <v>90.67</v>
+        <v>88.41</v>
       </c>
       <c r="S17" t="n">
-        <v>268.65</v>
+        <v>273.22</v>
       </c>
       <c r="T17" t="n">
-        <v>42.75</v>
+        <v>38.13</v>
       </c>
       <c r="U17" t="n">
-        <v>151.74</v>
+        <v>157.42</v>
       </c>
       <c r="V17" t="n">
-        <v>87.3</v>
+        <v>77.52</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>44713</v>
+        <v>44682</v>
       </c>
       <c r="B18" t="n">
-        <v>11028.74</v>
+        <v>12081.39</v>
       </c>
       <c r="C18" t="n">
-        <v>134.89</v>
+        <v>146.63</v>
       </c>
       <c r="D18" t="n">
-        <v>234.2</v>
+        <v>234.69</v>
       </c>
       <c r="E18" t="n">
-        <v>106.21</v>
+        <v>120.21</v>
       </c>
       <c r="F18" t="n">
-        <v>224.24</v>
+        <v>229.53</v>
       </c>
       <c r="G18" t="n">
-        <v>28.91</v>
+        <v>34.55</v>
       </c>
       <c r="H18" t="n">
-        <v>84.01000000000001</v>
+        <v>108.47</v>
       </c>
       <c r="I18" t="n">
-        <v>55.78</v>
+        <v>57.85</v>
       </c>
       <c r="J18" t="n">
-        <v>11.87</v>
+        <v>20.98</v>
       </c>
       <c r="K18" t="n">
-        <v>164.82</v>
+        <v>165.63</v>
       </c>
       <c r="L18" t="n">
-        <v>104.39</v>
+        <v>122.57</v>
       </c>
       <c r="M18" t="n">
-        <v>9.949999999999999</v>
+        <v>12.16</v>
       </c>
       <c r="N18" t="n">
-        <v>47.4</v>
+        <v>53.22</v>
       </c>
       <c r="O18" t="n">
-        <v>17.71</v>
+        <v>17.99</v>
       </c>
       <c r="P18" t="n">
-        <v>539.47</v>
+        <v>563.59</v>
       </c>
       <c r="Q18" t="n">
-        <v>224.47</v>
+        <v>252.75</v>
       </c>
       <c r="R18" t="n">
-        <v>77.77</v>
+        <v>90.67</v>
       </c>
       <c r="S18" t="n">
-        <v>281.79</v>
+        <v>268.65</v>
       </c>
       <c r="T18" t="n">
-        <v>42.3</v>
+        <v>42.75</v>
       </c>
       <c r="U18" t="n">
-        <v>146.45</v>
+        <v>151.74</v>
       </c>
       <c r="V18" t="n">
-        <v>78.68000000000001</v>
+        <v>87.3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>44743</v>
+        <v>44713</v>
       </c>
       <c r="B19" t="n">
-        <v>12390.69</v>
+        <v>11028.74</v>
       </c>
       <c r="C19" t="n">
-        <v>160.33</v>
+        <v>134.89</v>
       </c>
       <c r="D19" t="n">
-        <v>249.64</v>
+        <v>234.2</v>
       </c>
       <c r="E19" t="n">
-        <v>134.95</v>
+        <v>106.21</v>
       </c>
       <c r="F19" t="n">
-        <v>233.01</v>
+        <v>224.24</v>
       </c>
       <c r="G19" t="n">
-        <v>31.58</v>
+        <v>28.91</v>
       </c>
       <c r="H19" t="n">
-        <v>94</v>
+        <v>84.01000000000001</v>
       </c>
       <c r="I19" t="n">
-        <v>57.37</v>
+        <v>55.78</v>
       </c>
       <c r="J19" t="n">
-        <v>11</v>
+        <v>11.87</v>
       </c>
       <c r="K19" t="n">
-        <v>162.04</v>
+        <v>164.82</v>
       </c>
       <c r="L19" t="n">
-        <v>106.93</v>
+        <v>104.39</v>
       </c>
       <c r="M19" t="n">
-        <v>10.82</v>
+        <v>9.949999999999999</v>
       </c>
       <c r="N19" t="n">
-        <v>48.39</v>
+        <v>47.4</v>
       </c>
       <c r="O19" t="n">
-        <v>15.87</v>
+        <v>17.71</v>
       </c>
       <c r="P19" t="n">
-        <v>594.5599999999999</v>
+        <v>539.47</v>
       </c>
       <c r="Q19" t="n">
-        <v>297.15</v>
+        <v>224.47</v>
       </c>
       <c r="R19" t="n">
-        <v>84.62</v>
+        <v>77.77</v>
       </c>
       <c r="S19" t="n">
-        <v>280.41</v>
+        <v>281.79</v>
       </c>
       <c r="T19" t="n">
-        <v>38.5</v>
+        <v>42.3</v>
       </c>
       <c r="U19" t="n">
-        <v>158.18</v>
+        <v>146.45</v>
       </c>
       <c r="V19" t="n">
-        <v>89.05</v>
+        <v>78.68000000000001</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>44774</v>
+        <v>44743</v>
       </c>
       <c r="B20" t="n">
-        <v>11816.2</v>
+        <v>12390.69</v>
       </c>
       <c r="C20" t="n">
-        <v>155.11</v>
+        <v>160.33</v>
       </c>
       <c r="D20" t="n">
-        <v>234.18</v>
+        <v>249.64</v>
       </c>
       <c r="E20" t="n">
-        <v>126.77</v>
+        <v>134.95</v>
       </c>
       <c r="F20" t="n">
-        <v>236.98</v>
+        <v>233.01</v>
       </c>
       <c r="G20" t="n">
-        <v>31.39</v>
+        <v>31.58</v>
       </c>
       <c r="H20" t="n">
-        <v>87.59</v>
+        <v>94</v>
       </c>
       <c r="I20" t="n">
-        <v>58.92</v>
+        <v>57.37</v>
       </c>
       <c r="J20" t="n">
-        <v>14.76</v>
+        <v>11</v>
       </c>
       <c r="K20" t="n">
-        <v>149.8</v>
+        <v>162.04</v>
       </c>
       <c r="L20" t="n">
-        <v>106.36</v>
+        <v>106.93</v>
       </c>
       <c r="M20" t="n">
-        <v>12.29</v>
+        <v>10.82</v>
       </c>
       <c r="N20" t="n">
-        <v>48.03</v>
+        <v>48.39</v>
       </c>
       <c r="O20" t="n">
-        <v>15.02</v>
+        <v>15.87</v>
       </c>
       <c r="P20" t="n">
-        <v>541.8099999999999</v>
+        <v>594.5599999999999</v>
       </c>
       <c r="Q20" t="n">
-        <v>275.61</v>
+        <v>297.15</v>
       </c>
       <c r="R20" t="n">
-        <v>79.70999999999999</v>
+        <v>84.62</v>
       </c>
       <c r="S20" t="n">
-        <v>281.76</v>
+        <v>280.41</v>
       </c>
       <c r="T20" t="n">
-        <v>35.29</v>
+        <v>38.5</v>
       </c>
       <c r="U20" t="n">
-        <v>162.48</v>
+        <v>158.18</v>
       </c>
       <c r="V20" t="n">
-        <v>87.81999999999999</v>
+        <v>89.05</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>44805</v>
+        <v>44774</v>
       </c>
       <c r="B21" t="n">
-        <v>10575.62</v>
+        <v>11816.2</v>
       </c>
       <c r="C21" t="n">
-        <v>136.54</v>
+        <v>155.11</v>
       </c>
       <c r="D21" t="n">
-        <v>197.9</v>
+        <v>234.18</v>
       </c>
       <c r="E21" t="n">
-        <v>113</v>
+        <v>126.77</v>
       </c>
       <c r="F21" t="n">
-        <v>218.46</v>
+        <v>236.98</v>
       </c>
       <c r="G21" t="n">
-        <v>28.21</v>
+        <v>31.39</v>
       </c>
       <c r="H21" t="n">
-        <v>78.05</v>
+        <v>87.59</v>
       </c>
       <c r="I21" t="n">
-        <v>56.91</v>
+        <v>58.92</v>
       </c>
       <c r="J21" t="n">
-        <v>13.15</v>
+        <v>14.76</v>
       </c>
       <c r="K21" t="n">
-        <v>152.7</v>
+        <v>149.8</v>
       </c>
       <c r="L21" t="n">
-        <v>97.72</v>
+        <v>106.36</v>
       </c>
       <c r="M21" t="n">
-        <v>12.46</v>
+        <v>12.29</v>
       </c>
       <c r="N21" t="n">
-        <v>45.54</v>
+        <v>48.03</v>
       </c>
       <c r="O21" t="n">
-        <v>13.13</v>
+        <v>15.02</v>
       </c>
       <c r="P21" t="n">
-        <v>503.93</v>
+        <v>541.8099999999999</v>
       </c>
       <c r="Q21" t="n">
-        <v>265.25</v>
+        <v>275.61</v>
       </c>
       <c r="R21" t="n">
-        <v>65.56999999999999</v>
+        <v>79.70999999999999</v>
       </c>
       <c r="S21" t="n">
-        <v>289.54</v>
+        <v>281.76</v>
       </c>
       <c r="T21" t="n">
-        <v>32.04</v>
+        <v>35.29</v>
       </c>
       <c r="U21" t="n">
-        <v>154</v>
+        <v>162.48</v>
       </c>
       <c r="V21" t="n">
-        <v>80.98999999999999</v>
+        <v>87.81999999999999</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>44835</v>
+        <v>44805</v>
       </c>
       <c r="B22" t="n">
-        <v>10988.15</v>
+        <v>10575.62</v>
       </c>
       <c r="C22" t="n">
-        <v>151.49</v>
+        <v>136.54</v>
       </c>
       <c r="D22" t="n">
-        <v>190.98</v>
+        <v>197.9</v>
       </c>
       <c r="E22" t="n">
-        <v>102.44</v>
+        <v>113</v>
       </c>
       <c r="F22" t="n">
-        <v>236.71</v>
+        <v>218.46</v>
       </c>
       <c r="G22" t="n">
-        <v>33.89</v>
+        <v>28.21</v>
       </c>
       <c r="H22" t="n">
-        <v>84.98</v>
+        <v>78.05</v>
       </c>
       <c r="I22" t="n">
-        <v>52.11</v>
+        <v>56.91</v>
       </c>
       <c r="J22" t="n">
-        <v>16</v>
+        <v>13.15</v>
       </c>
       <c r="K22" t="n">
-        <v>162.62</v>
+        <v>152.7</v>
       </c>
       <c r="L22" t="n">
-        <v>117.72</v>
+        <v>97.72</v>
       </c>
       <c r="M22" t="n">
-        <v>14.88</v>
+        <v>12.46</v>
       </c>
       <c r="N22" t="n">
-        <v>50.91</v>
+        <v>45.54</v>
       </c>
       <c r="O22" t="n">
-        <v>15.61</v>
+        <v>13.13</v>
       </c>
       <c r="P22" t="n">
-        <v>510.94</v>
+        <v>503.93</v>
       </c>
       <c r="Q22" t="n">
-        <v>227.54</v>
+        <v>265.25</v>
       </c>
       <c r="R22" t="n">
-        <v>59.2</v>
+        <v>65.56999999999999</v>
       </c>
       <c r="S22" t="n">
-        <v>312</v>
+        <v>289.54</v>
       </c>
       <c r="T22" t="n">
-        <v>31.54</v>
+        <v>32.04</v>
       </c>
       <c r="U22" t="n">
-        <v>152.81</v>
+        <v>154</v>
       </c>
       <c r="V22" t="n">
-        <v>102.79</v>
+        <v>80.98999999999999</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>44866</v>
+        <v>44835</v>
       </c>
       <c r="B23" t="n">
-        <v>11468</v>
+        <v>10988.15</v>
       </c>
       <c r="C23" t="n">
-        <v>146.25</v>
+        <v>151.49</v>
       </c>
       <c r="D23" t="n">
-        <v>205.43</v>
+        <v>190.98</v>
       </c>
       <c r="E23" t="n">
-        <v>96.54000000000001</v>
+        <v>102.44</v>
       </c>
       <c r="F23" t="n">
-        <v>293.2</v>
+        <v>236.71</v>
       </c>
       <c r="G23" t="n">
-        <v>35.59</v>
+        <v>33.89</v>
       </c>
       <c r="H23" t="n">
-        <v>86.18000000000001</v>
+        <v>84.98</v>
       </c>
       <c r="I23" t="n">
-        <v>49.57</v>
+        <v>52.11</v>
       </c>
       <c r="J23" t="n">
-        <v>13.72</v>
+        <v>16</v>
       </c>
       <c r="K23" t="n">
-        <v>166.38</v>
+        <v>162.62</v>
       </c>
       <c r="L23" t="n">
-        <v>130.38</v>
+        <v>117.72</v>
       </c>
       <c r="M23" t="n">
-        <v>15.65</v>
+        <v>14.88</v>
       </c>
       <c r="N23" t="n">
-        <v>53.51</v>
+        <v>50.91</v>
       </c>
       <c r="O23" t="n">
-        <v>16.8</v>
+        <v>15.61</v>
       </c>
       <c r="P23" t="n">
-        <v>556.92</v>
+        <v>510.94</v>
       </c>
       <c r="Q23" t="n">
-        <v>194.7</v>
+        <v>227.54</v>
       </c>
       <c r="R23" t="n">
-        <v>79.81</v>
+        <v>59.2</v>
       </c>
       <c r="S23" t="n">
-        <v>316.4</v>
+        <v>312</v>
       </c>
       <c r="T23" t="n">
-        <v>33.45</v>
+        <v>31.54</v>
       </c>
       <c r="U23" t="n">
-        <v>161.83</v>
+        <v>152.81</v>
       </c>
       <c r="V23" t="n">
-        <v>103.28</v>
+        <v>102.79</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>44896</v>
+        <v>44866</v>
       </c>
       <c r="B24" t="n">
-        <v>10466.48</v>
+        <v>11468</v>
       </c>
       <c r="C24" t="n">
-        <v>128.58</v>
+        <v>146.25</v>
       </c>
       <c r="D24" t="n">
-        <v>196.71</v>
+        <v>205.43</v>
       </c>
       <c r="E24" t="n">
-        <v>84</v>
+        <v>96.54000000000001</v>
       </c>
       <c r="F24" t="n">
-        <v>291.4</v>
+        <v>293.2</v>
       </c>
       <c r="G24" t="n">
-        <v>31.14</v>
+        <v>35.59</v>
       </c>
       <c r="H24" t="n">
-        <v>69.84999999999999</v>
+        <v>86.18000000000001</v>
       </c>
       <c r="I24" t="n">
-        <v>52.84</v>
+        <v>49.57</v>
       </c>
       <c r="J24" t="n">
-        <v>12.3</v>
+        <v>13.72</v>
       </c>
       <c r="K24" t="n">
-        <v>166.19</v>
+        <v>166.38</v>
       </c>
       <c r="L24" t="n">
-        <v>126.53</v>
+        <v>130.38</v>
       </c>
       <c r="M24" t="n">
-        <v>16.2</v>
+        <v>15.65</v>
       </c>
       <c r="N24" t="n">
-        <v>52.58</v>
+        <v>53.51</v>
       </c>
       <c r="O24" t="n">
-        <v>16.04</v>
+        <v>16.8</v>
       </c>
       <c r="P24" t="n">
-        <v>547.4400000000001</v>
+        <v>556.92</v>
       </c>
       <c r="Q24" t="n">
-        <v>123.18</v>
+        <v>194.7</v>
       </c>
       <c r="R24" t="n">
-        <v>71.64</v>
+        <v>79.81</v>
       </c>
       <c r="S24" t="n">
-        <v>288.78</v>
+        <v>316.4</v>
       </c>
       <c r="T24" t="n">
-        <v>33.81</v>
+        <v>33.45</v>
       </c>
       <c r="U24" t="n">
-        <v>151.37</v>
+        <v>161.83</v>
       </c>
       <c r="V24" t="n">
-        <v>103.14</v>
+        <v>103.28</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>44927</v>
+        <v>44896</v>
       </c>
       <c r="B25" t="n">
-        <v>11584.55</v>
+        <v>10466.48</v>
       </c>
       <c r="C25" t="n">
-        <v>142.79</v>
+        <v>128.58</v>
       </c>
       <c r="D25" t="n">
-        <v>208.95</v>
+        <v>196.71</v>
       </c>
       <c r="E25" t="n">
-        <v>103.13</v>
+        <v>84</v>
       </c>
       <c r="F25" t="n">
-        <v>304.57</v>
+        <v>291.4</v>
       </c>
       <c r="G25" t="n">
-        <v>33.55</v>
+        <v>31.14</v>
       </c>
       <c r="H25" t="n">
-        <v>90.34999999999999</v>
+        <v>69.84999999999999</v>
       </c>
       <c r="I25" t="n">
-        <v>50.07</v>
+        <v>52.84</v>
       </c>
       <c r="J25" t="n">
-        <v>13.19</v>
+        <v>12.3</v>
       </c>
       <c r="K25" t="n">
-        <v>153.74</v>
+        <v>166.19</v>
       </c>
       <c r="L25" t="n">
-        <v>132.06</v>
+        <v>126.53</v>
       </c>
       <c r="M25" t="n">
-        <v>15.84</v>
+        <v>16.2</v>
       </c>
       <c r="N25" t="n">
-        <v>54.3</v>
+        <v>52.58</v>
       </c>
       <c r="O25" t="n">
-        <v>17.75</v>
+        <v>16.04</v>
       </c>
       <c r="P25" t="n">
-        <v>567.26</v>
+        <v>547.4400000000001</v>
       </c>
       <c r="Q25" t="n">
-        <v>173.22</v>
+        <v>123.18</v>
       </c>
       <c r="R25" t="n">
-        <v>89.69</v>
+        <v>71.64</v>
       </c>
       <c r="S25" t="n">
-        <v>323.1</v>
+        <v>288.78</v>
       </c>
       <c r="T25" t="n">
-        <v>35.67</v>
+        <v>33.81</v>
       </c>
       <c r="U25" t="n">
-        <v>149.87</v>
+        <v>151.37</v>
       </c>
       <c r="V25" t="n">
-        <v>108.48</v>
+        <v>103.14</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>44958</v>
+        <v>44927</v>
       </c>
       <c r="B26" t="n">
-        <v>11455.54</v>
+        <v>11584.55</v>
       </c>
       <c r="C26" t="n">
-        <v>145.88</v>
+        <v>142.79</v>
       </c>
       <c r="D26" t="n">
-        <v>185.21</v>
+        <v>208.95</v>
       </c>
       <c r="E26" t="n">
-        <v>94.23</v>
+        <v>103.13</v>
       </c>
       <c r="F26" t="n">
-        <v>271.75</v>
+        <v>304.57</v>
       </c>
       <c r="G26" t="n">
-        <v>32.44</v>
+        <v>33.55</v>
       </c>
       <c r="H26" t="n">
-        <v>85.48999999999999</v>
+        <v>90.34999999999999</v>
       </c>
       <c r="I26" t="n">
-        <v>51.91</v>
+        <v>50.07</v>
       </c>
       <c r="J26" t="n">
-        <v>13</v>
+        <v>13.19</v>
       </c>
       <c r="K26" t="n">
-        <v>144.18</v>
+        <v>153.74</v>
       </c>
       <c r="L26" t="n">
-        <v>136.25</v>
+        <v>132.06</v>
       </c>
       <c r="M26" t="n">
-        <v>15.57</v>
+        <v>15.84</v>
       </c>
       <c r="N26" t="n">
-        <v>56.11</v>
+        <v>54.3</v>
       </c>
       <c r="O26" t="n">
-        <v>16.72</v>
+        <v>17.75</v>
       </c>
       <c r="P26" t="n">
-        <v>538.85</v>
+        <v>567.26</v>
       </c>
       <c r="Q26" t="n">
-        <v>205.71</v>
+        <v>173.22</v>
       </c>
       <c r="R26" t="n">
-        <v>84.22</v>
+        <v>89.69</v>
       </c>
       <c r="S26" t="n">
-        <v>290.29</v>
+        <v>323.1</v>
       </c>
       <c r="T26" t="n">
-        <v>33.83</v>
+        <v>35.67</v>
       </c>
       <c r="U26" t="n">
-        <v>145.06</v>
+        <v>149.87</v>
       </c>
       <c r="V26" t="n">
-        <v>102.78</v>
+        <v>108.48</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>44986</v>
+        <v>44958</v>
       </c>
       <c r="B27" t="n">
-        <v>12221.91</v>
+        <v>11455.54</v>
       </c>
       <c r="C27" t="n">
-        <v>163.43</v>
+        <v>145.88</v>
       </c>
       <c r="D27" t="n">
-        <v>191.13</v>
+        <v>185.21</v>
       </c>
       <c r="E27" t="n">
-        <v>103.29</v>
+        <v>94.23</v>
       </c>
       <c r="F27" t="n">
-        <v>272.92</v>
+        <v>271.75</v>
       </c>
       <c r="G27" t="n">
-        <v>27.05</v>
+        <v>32.44</v>
       </c>
       <c r="H27" t="n">
-        <v>83.45999999999999</v>
+        <v>85.48999999999999</v>
       </c>
       <c r="I27" t="n">
-        <v>52.43</v>
+        <v>51.91</v>
       </c>
       <c r="J27" t="n">
-        <v>12.41</v>
+        <v>13</v>
       </c>
       <c r="K27" t="n">
-        <v>146.87</v>
+        <v>144.18</v>
       </c>
       <c r="L27" t="n">
-        <v>123.86</v>
+        <v>136.25</v>
       </c>
       <c r="M27" t="n">
-        <v>16.11</v>
+        <v>15.57</v>
       </c>
       <c r="N27" t="n">
-        <v>53.62</v>
+        <v>56.11</v>
       </c>
       <c r="O27" t="n">
-        <v>17.02</v>
+        <v>16.72</v>
       </c>
       <c r="P27" t="n">
-        <v>573.27</v>
+        <v>538.85</v>
       </c>
       <c r="Q27" t="n">
-        <v>207.46</v>
+        <v>205.71</v>
       </c>
       <c r="R27" t="n">
-        <v>89.97</v>
+        <v>84.22</v>
       </c>
       <c r="S27" t="n">
-        <v>315.07</v>
+        <v>290.29</v>
       </c>
       <c r="T27" t="n">
-        <v>33.9</v>
+        <v>33.83</v>
       </c>
       <c r="U27" t="n">
-        <v>158.05</v>
+        <v>145.06</v>
       </c>
       <c r="V27" t="n">
-        <v>103.33</v>
+        <v>102.78</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45017</v>
+        <v>44986</v>
       </c>
       <c r="B28" t="n">
-        <v>12226.58</v>
+        <v>12221.91</v>
       </c>
       <c r="C28" t="n">
-        <v>168.17</v>
+        <v>163.43</v>
       </c>
       <c r="D28" t="n">
-        <v>191.18</v>
+        <v>191.13</v>
       </c>
       <c r="E28" t="n">
-        <v>105.45</v>
+        <v>103.29</v>
       </c>
       <c r="F28" t="n">
-        <v>281.48</v>
+        <v>272.92</v>
       </c>
       <c r="G28" t="n">
-        <v>27.87</v>
+        <v>27.05</v>
       </c>
       <c r="H28" t="n">
-        <v>84.88</v>
+        <v>83.45999999999999</v>
       </c>
       <c r="I28" t="n">
-        <v>57.05</v>
+        <v>52.43</v>
       </c>
       <c r="J28" t="n">
-        <v>10.85</v>
+        <v>12.41</v>
       </c>
       <c r="K28" t="n">
-        <v>155.11</v>
+        <v>146.87</v>
       </c>
       <c r="L28" t="n">
-        <v>131.4</v>
+        <v>123.86</v>
       </c>
       <c r="M28" t="n">
-        <v>17.05</v>
+        <v>16.11</v>
       </c>
       <c r="N28" t="n">
-        <v>57.76</v>
+        <v>53.62</v>
       </c>
       <c r="O28" t="n">
-        <v>15.62</v>
+        <v>17.02</v>
       </c>
       <c r="P28" t="n">
-        <v>552.27</v>
+        <v>573.27</v>
       </c>
       <c r="Q28" t="n">
-        <v>164.31</v>
+        <v>207.46</v>
       </c>
       <c r="R28" t="n">
-        <v>81.95999999999999</v>
+        <v>89.97</v>
       </c>
       <c r="S28" t="n">
-        <v>340.73</v>
+        <v>315.07</v>
       </c>
       <c r="T28" t="n">
-        <v>33.85</v>
+        <v>33.9</v>
       </c>
       <c r="U28" t="n">
-        <v>161.59</v>
+        <v>158.05</v>
       </c>
       <c r="V28" t="n">
-        <v>111.51</v>
+        <v>103.33</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45047</v>
+        <v>45017</v>
       </c>
       <c r="B29" t="n">
-        <v>12935.29</v>
+        <v>12226.58</v>
       </c>
       <c r="C29" t="n">
-        <v>175.67</v>
+        <v>168.17</v>
       </c>
       <c r="D29" t="n">
-        <v>173.8</v>
+        <v>191.18</v>
       </c>
       <c r="E29" t="n">
-        <v>120.58</v>
+        <v>105.45</v>
       </c>
       <c r="F29" t="n">
-        <v>257.36</v>
+        <v>281.48</v>
       </c>
       <c r="G29" t="n">
-        <v>26.45</v>
+        <v>27.87</v>
       </c>
       <c r="H29" t="n">
-        <v>82.15000000000001</v>
+        <v>84.88</v>
       </c>
       <c r="I29" t="n">
-        <v>50.87</v>
+        <v>57.05</v>
       </c>
       <c r="J29" t="n">
-        <v>9.460000000000001</v>
+        <v>10.85</v>
       </c>
       <c r="K29" t="n">
-        <v>146.92</v>
+        <v>155.11</v>
       </c>
       <c r="L29" t="n">
-        <v>130.01</v>
+        <v>131.4</v>
       </c>
       <c r="M29" t="n">
-        <v>16.88</v>
+        <v>17.05</v>
       </c>
       <c r="N29" t="n">
-        <v>52.19</v>
+        <v>57.76</v>
       </c>
       <c r="O29" t="n">
-        <v>14.1</v>
+        <v>15.62</v>
       </c>
       <c r="P29" t="n">
-        <v>506.05</v>
+        <v>552.27</v>
       </c>
       <c r="Q29" t="n">
-        <v>203.93</v>
+        <v>164.31</v>
       </c>
       <c r="R29" t="n">
-        <v>95.86</v>
+        <v>81.95999999999999</v>
       </c>
       <c r="S29" t="n">
-        <v>323.57</v>
+        <v>340.73</v>
       </c>
       <c r="T29" t="n">
-        <v>31.57</v>
+        <v>33.85</v>
       </c>
       <c r="U29" t="n">
-        <v>157.57</v>
+        <v>161.59</v>
       </c>
       <c r="V29" t="n">
-        <v>96.28</v>
+        <v>111.51</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45078</v>
+        <v>45047</v>
       </c>
       <c r="B30" t="n">
-        <v>13787.92</v>
+        <v>12935.29</v>
       </c>
       <c r="C30" t="n">
-        <v>192.51</v>
+        <v>175.67</v>
       </c>
       <c r="D30" t="n">
-        <v>182.75</v>
+        <v>173.8</v>
       </c>
       <c r="E30" t="n">
-        <v>130.36</v>
+        <v>120.58</v>
       </c>
       <c r="F30" t="n">
-        <v>286.42</v>
+        <v>257.36</v>
       </c>
       <c r="G30" t="n">
-        <v>27.31</v>
+        <v>26.45</v>
       </c>
       <c r="H30" t="n">
-        <v>89.18000000000001</v>
+        <v>82.15000000000001</v>
       </c>
       <c r="I30" t="n">
-        <v>55.62</v>
+        <v>50.87</v>
       </c>
       <c r="J30" t="n">
-        <v>9.1</v>
+        <v>9.460000000000001</v>
       </c>
       <c r="K30" t="n">
-        <v>158.02</v>
+        <v>146.92</v>
       </c>
       <c r="L30" t="n">
-        <v>139.33</v>
+        <v>130.01</v>
       </c>
       <c r="M30" t="n">
-        <v>17.22</v>
+        <v>16.88</v>
       </c>
       <c r="N30" t="n">
-        <v>56.81</v>
+        <v>52.19</v>
       </c>
       <c r="O30" t="n">
-        <v>14.3</v>
+        <v>14.1</v>
       </c>
       <c r="P30" t="n">
-        <v>519.28</v>
+        <v>506.05</v>
       </c>
       <c r="Q30" t="n">
-        <v>261.77</v>
+        <v>203.93</v>
       </c>
       <c r="R30" t="n">
-        <v>98.12</v>
+        <v>95.86</v>
       </c>
       <c r="S30" t="n">
-        <v>351.91</v>
+        <v>323.57</v>
       </c>
       <c r="T30" t="n">
-        <v>32.95</v>
+        <v>31.57</v>
       </c>
       <c r="U30" t="n">
-        <v>168.77</v>
+        <v>157.57</v>
       </c>
       <c r="V30" t="n">
-        <v>101.94</v>
+        <v>96.28</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45108</v>
+        <v>45078</v>
       </c>
       <c r="B31" t="n">
-        <v>14346.02</v>
+        <v>13787.92</v>
       </c>
       <c r="C31" t="n">
-        <v>194.97</v>
+        <v>192.51</v>
       </c>
       <c r="D31" t="n">
-        <v>180.8</v>
+        <v>182.75</v>
       </c>
       <c r="E31" t="n">
-        <v>133.68</v>
+        <v>130.36</v>
       </c>
       <c r="F31" t="n">
-        <v>293.71</v>
+        <v>286.42</v>
       </c>
       <c r="G31" t="n">
-        <v>30.7</v>
+        <v>27.31</v>
       </c>
       <c r="H31" t="n">
-        <v>100.51</v>
+        <v>89.18000000000001</v>
       </c>
       <c r="I31" t="n">
-        <v>54.58</v>
+        <v>55.62</v>
       </c>
       <c r="J31" t="n">
-        <v>9</v>
+        <v>9.1</v>
       </c>
       <c r="K31" t="n">
-        <v>159.94</v>
+        <v>158.02</v>
       </c>
       <c r="L31" t="n">
-        <v>151.32</v>
+        <v>139.33</v>
       </c>
       <c r="M31" t="n">
-        <v>17.55</v>
+        <v>17.22</v>
       </c>
       <c r="N31" t="n">
-        <v>57.98</v>
+        <v>56.81</v>
       </c>
       <c r="O31" t="n">
-        <v>13.02</v>
+        <v>14.3</v>
       </c>
       <c r="P31" t="n">
-        <v>546.4299999999999</v>
+        <v>519.28</v>
       </c>
       <c r="Q31" t="n">
-        <v>267.43</v>
+        <v>261.77</v>
       </c>
       <c r="R31" t="n">
-        <v>96.8</v>
+        <v>98.12</v>
       </c>
       <c r="S31" t="n">
-        <v>352.34</v>
+        <v>351.91</v>
       </c>
       <c r="T31" t="n">
-        <v>30.2</v>
+        <v>32.95</v>
       </c>
       <c r="U31" t="n">
-        <v>160.09</v>
+        <v>168.77</v>
       </c>
       <c r="V31" t="n">
-        <v>101.93</v>
+        <v>101.94</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45139</v>
+        <v>45108</v>
       </c>
       <c r="B32" t="n">
-        <v>14034.97</v>
+        <v>14346.02</v>
       </c>
       <c r="C32" t="n">
-        <v>186.46</v>
+        <v>194.97</v>
       </c>
       <c r="D32" t="n">
-        <v>172.26</v>
+        <v>180.8</v>
       </c>
       <c r="E32" t="n">
-        <v>138.01</v>
+        <v>133.68</v>
       </c>
       <c r="F32" t="n">
-        <v>284.25</v>
+        <v>293.71</v>
       </c>
       <c r="G32" t="n">
-        <v>27.51</v>
+        <v>30.7</v>
       </c>
       <c r="H32" t="n">
-        <v>102.82</v>
+        <v>100.51</v>
       </c>
       <c r="I32" t="n">
-        <v>51.85</v>
+        <v>54.58</v>
       </c>
       <c r="J32" t="n">
-        <v>8.74</v>
+        <v>9</v>
       </c>
       <c r="K32" t="n">
-        <v>154.35</v>
+        <v>159.94</v>
       </c>
       <c r="L32" t="n">
-        <v>141.14</v>
+        <v>151.32</v>
       </c>
       <c r="M32" t="n">
-        <v>16.24</v>
+        <v>17.55</v>
       </c>
       <c r="N32" t="n">
-        <v>58.41</v>
+        <v>57.98</v>
       </c>
       <c r="O32" t="n">
-        <v>13.5</v>
+        <v>13.02</v>
       </c>
       <c r="P32" t="n">
-        <v>554.83</v>
+        <v>546.4299999999999</v>
       </c>
       <c r="Q32" t="n">
-        <v>258.08</v>
+        <v>267.43</v>
       </c>
       <c r="R32" t="n">
-        <v>91.36</v>
+        <v>96.8</v>
       </c>
       <c r="S32" t="n">
-        <v>348.34</v>
+        <v>352.34</v>
       </c>
       <c r="T32" t="n">
-        <v>31.55</v>
+        <v>30.2</v>
       </c>
       <c r="U32" t="n">
-        <v>153.24</v>
+        <v>160.09</v>
       </c>
       <c r="V32" t="n">
-        <v>105.68</v>
+        <v>101.93</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45170</v>
+        <v>45139</v>
       </c>
       <c r="B33" t="n">
-        <v>13219.32</v>
+        <v>14034.97</v>
       </c>
       <c r="C33" t="n">
-        <v>170.15</v>
+        <v>186.46</v>
       </c>
       <c r="D33" t="n">
-        <v>156.24</v>
+        <v>172.26</v>
       </c>
       <c r="E33" t="n">
-        <v>127.12</v>
+        <v>138.01</v>
       </c>
       <c r="F33" t="n">
-        <v>272.62</v>
+        <v>284.25</v>
       </c>
       <c r="G33" t="n">
-        <v>26.49</v>
+        <v>27.51</v>
       </c>
       <c r="H33" t="n">
-        <v>103.56</v>
+        <v>102.82</v>
       </c>
       <c r="I33" t="n">
-        <v>51.9</v>
+        <v>51.85</v>
       </c>
       <c r="J33" t="n">
-        <v>9.630000000000001</v>
+        <v>8.74</v>
       </c>
       <c r="K33" t="n">
-        <v>149.77</v>
+        <v>154.35</v>
       </c>
       <c r="L33" t="n">
-        <v>139.88</v>
+        <v>141.14</v>
       </c>
       <c r="M33" t="n">
-        <v>16.07</v>
+        <v>16.24</v>
       </c>
       <c r="N33" t="n">
-        <v>61.22</v>
+        <v>58.41</v>
       </c>
       <c r="O33" t="n">
-        <v>13.71</v>
+        <v>13.5</v>
       </c>
       <c r="P33" t="n">
-        <v>504.11</v>
+        <v>554.83</v>
       </c>
       <c r="Q33" t="n">
-        <v>250.22</v>
+        <v>258.08</v>
       </c>
       <c r="R33" t="n">
-        <v>84.84</v>
+        <v>91.36</v>
       </c>
       <c r="S33" t="n">
-        <v>347.74</v>
+        <v>348.34</v>
       </c>
       <c r="T33" t="n">
-        <v>29.23</v>
+        <v>31.55</v>
       </c>
       <c r="U33" t="n">
-        <v>148.99</v>
+        <v>153.24</v>
       </c>
       <c r="V33" t="n">
-        <v>112.67</v>
+        <v>105.68</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45200</v>
+        <v>45170</v>
       </c>
       <c r="B34" t="n">
-        <v>12851.24</v>
+        <v>13219.32</v>
       </c>
       <c r="C34" t="n">
-        <v>169.71</v>
+        <v>170.15</v>
       </c>
       <c r="D34" t="n">
-        <v>169.29</v>
+        <v>156.24</v>
       </c>
       <c r="E34" t="n">
-        <v>133.09</v>
+        <v>127.12</v>
       </c>
       <c r="F34" t="n">
-        <v>273.36</v>
+        <v>272.62</v>
       </c>
       <c r="G34" t="n">
-        <v>25.48</v>
+        <v>26.49</v>
       </c>
       <c r="H34" t="n">
-        <v>89.26000000000001</v>
+        <v>103.56</v>
       </c>
       <c r="I34" t="n">
-        <v>50.73</v>
+        <v>51.9</v>
       </c>
       <c r="J34" t="n">
-        <v>8.359999999999999</v>
+        <v>9.630000000000001</v>
       </c>
       <c r="K34" t="n">
-        <v>142.65</v>
+        <v>149.77</v>
       </c>
       <c r="L34" t="n">
-        <v>134.13</v>
+        <v>139.88</v>
       </c>
       <c r="M34" t="n">
-        <v>16.24</v>
+        <v>16.07</v>
       </c>
       <c r="N34" t="n">
-        <v>61.94</v>
+        <v>61.22</v>
       </c>
       <c r="O34" t="n">
-        <v>14.05</v>
+        <v>13.71</v>
       </c>
       <c r="P34" t="n">
-        <v>443.26</v>
+        <v>504.11</v>
       </c>
       <c r="Q34" t="n">
-        <v>200.84</v>
+        <v>250.22</v>
       </c>
       <c r="R34" t="n">
-        <v>84.70999999999999</v>
+        <v>84.84</v>
       </c>
       <c r="S34" t="n">
-        <v>362.11</v>
+        <v>347.74</v>
       </c>
       <c r="T34" t="n">
-        <v>31.69</v>
+        <v>29.23</v>
       </c>
       <c r="U34" t="n">
-        <v>161.34</v>
+        <v>148.99</v>
       </c>
       <c r="V34" t="n">
-        <v>101.43</v>
+        <v>112.67</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45231</v>
+        <v>45200</v>
       </c>
       <c r="B35" t="n">
-        <v>14226.22</v>
+        <v>12851.24</v>
       </c>
       <c r="C35" t="n">
-        <v>188.78</v>
+        <v>169.71</v>
       </c>
       <c r="D35" t="n">
-        <v>200.35</v>
+        <v>169.29</v>
       </c>
       <c r="E35" t="n">
-        <v>146.09</v>
+        <v>133.09</v>
       </c>
       <c r="F35" t="n">
-        <v>261.85</v>
+        <v>273.36</v>
       </c>
       <c r="G35" t="n">
-        <v>29.5</v>
+        <v>25.48</v>
       </c>
       <c r="H35" t="n">
-        <v>109.56</v>
+        <v>89.26000000000001</v>
       </c>
       <c r="I35" t="n">
-        <v>52.4</v>
+        <v>50.73</v>
       </c>
       <c r="J35" t="n">
-        <v>9.039999999999999</v>
+        <v>8.359999999999999</v>
       </c>
       <c r="K35" t="n">
-        <v>148.72</v>
+        <v>142.65</v>
       </c>
       <c r="L35" t="n">
-        <v>151.66</v>
+        <v>134.13</v>
       </c>
       <c r="M35" t="n">
-        <v>17.11</v>
+        <v>16.24</v>
       </c>
       <c r="N35" t="n">
-        <v>62.57</v>
+        <v>61.94</v>
       </c>
       <c r="O35" t="n">
-        <v>15.41</v>
+        <v>14.05</v>
       </c>
       <c r="P35" t="n">
-        <v>494.08</v>
+        <v>443.26</v>
       </c>
       <c r="Q35" t="n">
-        <v>240.08</v>
+        <v>200.84</v>
       </c>
       <c r="R35" t="n">
-        <v>95.5</v>
+        <v>84.70999999999999</v>
       </c>
       <c r="S35" t="n">
-        <v>354.81</v>
+        <v>362.11</v>
       </c>
       <c r="T35" t="n">
-        <v>35.31</v>
+        <v>31.69</v>
       </c>
       <c r="U35" t="n">
-        <v>167.88</v>
+        <v>161.34</v>
       </c>
       <c r="V35" t="n">
-        <v>98.45</v>
+        <v>101.43</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45261</v>
+        <v>45231</v>
       </c>
       <c r="B36" t="n">
-        <v>15011.35</v>
+        <v>14226.22</v>
       </c>
       <c r="C36" t="n">
-        <v>191.59</v>
+        <v>188.78</v>
       </c>
       <c r="D36" t="n">
-        <v>207.17</v>
+        <v>200.35</v>
       </c>
       <c r="E36" t="n">
-        <v>151.94</v>
+        <v>146.09</v>
       </c>
       <c r="F36" t="n">
-        <v>265</v>
+        <v>261.85</v>
       </c>
       <c r="G36" t="n">
-        <v>32.83</v>
+        <v>29.5</v>
       </c>
       <c r="H36" t="n">
-        <v>127.65</v>
+        <v>109.56</v>
       </c>
       <c r="I36" t="n">
-        <v>54.78</v>
+        <v>52.4</v>
       </c>
       <c r="J36" t="n">
-        <v>10.99</v>
+        <v>9.039999999999999</v>
       </c>
       <c r="K36" t="n">
-        <v>151.93</v>
+        <v>148.72</v>
       </c>
       <c r="L36" t="n">
-        <v>165.28</v>
+        <v>151.66</v>
       </c>
       <c r="M36" t="n">
-        <v>17.97</v>
+        <v>17.11</v>
       </c>
       <c r="N36" t="n">
-        <v>63.2</v>
+        <v>62.57</v>
       </c>
       <c r="O36" t="n">
-        <v>15.6</v>
+        <v>15.41</v>
       </c>
       <c r="P36" t="n">
-        <v>528.99</v>
+        <v>494.08</v>
       </c>
       <c r="Q36" t="n">
-        <v>248.48</v>
+        <v>240.08</v>
       </c>
       <c r="R36" t="n">
-        <v>102.07</v>
+        <v>95.5</v>
       </c>
       <c r="S36" t="n">
-        <v>406.89</v>
+        <v>354.81</v>
       </c>
       <c r="T36" t="n">
-        <v>34.73</v>
+        <v>35.31</v>
       </c>
       <c r="U36" t="n">
-        <v>176.57</v>
+        <v>167.88</v>
       </c>
       <c r="V36" t="n">
-        <v>96.68000000000001</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45292</v>
+        <v>45261</v>
       </c>
       <c r="B37" t="n">
-        <v>15164.01</v>
+        <v>15011.35</v>
       </c>
       <c r="C37" t="n">
-        <v>183.5</v>
+        <v>191.59</v>
       </c>
       <c r="D37" t="n">
-        <v>189.24</v>
+        <v>207.17</v>
       </c>
       <c r="E37" t="n">
-        <v>155.2</v>
+        <v>151.94</v>
       </c>
       <c r="F37" t="n">
-        <v>249.08</v>
+        <v>265</v>
       </c>
       <c r="G37" t="n">
-        <v>33.17</v>
+        <v>32.83</v>
       </c>
       <c r="H37" t="n">
-        <v>121.34</v>
+        <v>127.65</v>
       </c>
       <c r="I37" t="n">
-        <v>53.25</v>
+        <v>54.78</v>
       </c>
       <c r="J37" t="n">
-        <v>6.68</v>
+        <v>10.99</v>
       </c>
       <c r="K37" t="n">
-        <v>154.02</v>
+        <v>151.93</v>
       </c>
       <c r="L37" t="n">
-        <v>169.42</v>
+        <v>165.28</v>
       </c>
       <c r="M37" t="n">
-        <v>16.82</v>
+        <v>17.97</v>
       </c>
       <c r="N37" t="n">
-        <v>60.43</v>
+        <v>63.2</v>
       </c>
       <c r="O37" t="n">
-        <v>16.45</v>
+        <v>15.6</v>
       </c>
       <c r="P37" t="n">
-        <v>537.52</v>
+        <v>528.99</v>
       </c>
       <c r="Q37" t="n">
-        <v>187.29</v>
+        <v>248.48</v>
       </c>
       <c r="R37" t="n">
-        <v>111.38</v>
+        <v>102.07</v>
       </c>
       <c r="S37" t="n">
-        <v>433.38</v>
+        <v>406.89</v>
       </c>
       <c r="T37" t="n">
-        <v>39.01</v>
+        <v>34.73</v>
       </c>
       <c r="U37" t="n">
-        <v>183.01</v>
+        <v>176.57</v>
       </c>
       <c r="V37" t="n">
-        <v>99.42</v>
+        <v>96.68000000000001</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45323</v>
+        <v>45292</v>
       </c>
       <c r="B38" t="n">
-        <v>16091.92</v>
+        <v>15164.01</v>
       </c>
       <c r="C38" t="n">
-        <v>179.87</v>
+        <v>183.5</v>
       </c>
       <c r="D38" t="n">
-        <v>192.35</v>
+        <v>189.24</v>
       </c>
       <c r="E38" t="n">
-        <v>176.76</v>
+        <v>155.2</v>
       </c>
       <c r="F38" t="n">
-        <v>227.97</v>
+        <v>249.08</v>
       </c>
       <c r="G38" t="n">
-        <v>33.66</v>
+        <v>33.17</v>
       </c>
       <c r="H38" t="n">
-        <v>124.63</v>
+        <v>121.34</v>
       </c>
       <c r="I38" t="n">
-        <v>53.21</v>
+        <v>53.25</v>
       </c>
       <c r="J38" t="n">
-        <v>5.93</v>
+        <v>6.68</v>
       </c>
       <c r="K38" t="n">
-        <v>156.43</v>
+        <v>154.02</v>
       </c>
       <c r="L38" t="n">
-        <v>181.9</v>
+        <v>169.42</v>
       </c>
       <c r="M38" t="n">
-        <v>16.64</v>
+        <v>16.82</v>
       </c>
       <c r="N38" t="n">
-        <v>60.35</v>
+        <v>60.43</v>
       </c>
       <c r="O38" t="n">
-        <v>16</v>
+        <v>16.45</v>
       </c>
       <c r="P38" t="n">
-        <v>568.63</v>
+        <v>537.52</v>
       </c>
       <c r="Q38" t="n">
-        <v>201.88</v>
+        <v>187.29</v>
       </c>
       <c r="R38" t="n">
-        <v>126.87</v>
+        <v>111.38</v>
       </c>
       <c r="S38" t="n">
-        <v>420.74</v>
+        <v>433.38</v>
       </c>
       <c r="T38" t="n">
-        <v>37.49</v>
+        <v>39.01</v>
       </c>
       <c r="U38" t="n">
-        <v>202.74</v>
+        <v>183.01</v>
       </c>
       <c r="V38" t="n">
-        <v>101.07</v>
+        <v>99.42</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45352</v>
+        <v>45323</v>
       </c>
       <c r="B39" t="n">
-        <v>16379.46</v>
+        <v>16091.92</v>
       </c>
       <c r="C39" t="n">
-        <v>170.86</v>
+        <v>179.87</v>
       </c>
       <c r="D39" t="n">
-        <v>191.12</v>
+        <v>192.35</v>
       </c>
       <c r="E39" t="n">
-        <v>180.38</v>
+        <v>176.76</v>
       </c>
       <c r="F39" t="n">
-        <v>235.99</v>
+        <v>227.97</v>
       </c>
       <c r="G39" t="n">
-        <v>37.24</v>
+        <v>33.66</v>
       </c>
       <c r="H39" t="n">
-        <v>129.07</v>
+        <v>124.63</v>
       </c>
       <c r="I39" t="n">
-        <v>54.17</v>
+        <v>53.21</v>
       </c>
       <c r="J39" t="n">
-        <v>5.11</v>
+        <v>5.93</v>
       </c>
       <c r="K39" t="n">
-        <v>154.5</v>
+        <v>156.43</v>
       </c>
       <c r="L39" t="n">
-        <v>195.82</v>
+        <v>181.9</v>
       </c>
       <c r="M39" t="n">
-        <v>16.71</v>
+        <v>16.64</v>
       </c>
       <c r="N39" t="n">
-        <v>65.09999999999999</v>
+        <v>60.35</v>
       </c>
       <c r="O39" t="n">
-        <v>16.63</v>
+        <v>16</v>
       </c>
       <c r="P39" t="n">
-        <v>579.63</v>
+        <v>568.63</v>
       </c>
       <c r="Q39" t="n">
-        <v>175.79</v>
+        <v>201.88</v>
       </c>
       <c r="R39" t="n">
-        <v>134.15</v>
+        <v>126.87</v>
       </c>
       <c r="S39" t="n">
-        <v>418.01</v>
+        <v>420.74</v>
       </c>
       <c r="T39" t="n">
-        <v>39.31</v>
+        <v>37.49</v>
       </c>
       <c r="U39" t="n">
-        <v>210.14</v>
+        <v>202.74</v>
       </c>
       <c r="V39" t="n">
-        <v>113.45</v>
+        <v>101.07</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45383</v>
+        <v>45352</v>
       </c>
       <c r="B40" t="n">
-        <v>15657.82</v>
+        <v>16379.46</v>
       </c>
       <c r="C40" t="n">
-        <v>169.72</v>
+        <v>170.86</v>
       </c>
       <c r="D40" t="n">
-        <v>165.94</v>
+        <v>191.12</v>
       </c>
       <c r="E40" t="n">
-        <v>175</v>
+        <v>180.38</v>
       </c>
       <c r="F40" t="n">
-        <v>231.9</v>
+        <v>235.99</v>
       </c>
       <c r="G40" t="n">
-        <v>36.35</v>
+        <v>37.24</v>
       </c>
       <c r="H40" t="n">
-        <v>114.57</v>
+        <v>129.07</v>
       </c>
       <c r="I40" t="n">
-        <v>54</v>
+        <v>54.17</v>
       </c>
       <c r="J40" t="n">
-        <v>5.18</v>
+        <v>5.11</v>
       </c>
       <c r="K40" t="n">
-        <v>141.22</v>
+        <v>154.5</v>
       </c>
       <c r="L40" t="n">
-        <v>187.45</v>
+        <v>195.82</v>
       </c>
       <c r="M40" t="n">
-        <v>17.07</v>
+        <v>16.71</v>
       </c>
       <c r="N40" t="n">
-        <v>69.58</v>
+        <v>65.09999999999999</v>
       </c>
       <c r="O40" t="n">
-        <v>15.96</v>
+        <v>16.63</v>
       </c>
       <c r="P40" t="n">
-        <v>567.55</v>
+        <v>579.63</v>
       </c>
       <c r="Q40" t="n">
-        <v>183.28</v>
+        <v>175.79</v>
       </c>
       <c r="R40" t="n">
-        <v>135.97</v>
+        <v>134.15</v>
       </c>
       <c r="S40" t="n">
-        <v>392.81</v>
+        <v>418.01</v>
       </c>
       <c r="T40" t="n">
-        <v>36.99</v>
+        <v>39.31</v>
       </c>
       <c r="U40" t="n">
-        <v>205.81</v>
+        <v>210.14</v>
       </c>
       <c r="V40" t="n">
-        <v>115.43</v>
+        <v>113.45</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45413</v>
+        <v>45383</v>
       </c>
       <c r="B41" t="n">
-        <v>16735.02</v>
+        <v>15657.82</v>
       </c>
       <c r="C41" t="n">
-        <v>191.56</v>
+        <v>169.72</v>
       </c>
       <c r="D41" t="n">
-        <v>191.03</v>
+        <v>165.94</v>
       </c>
       <c r="E41" t="n">
-        <v>176.44</v>
+        <v>175</v>
       </c>
       <c r="F41" t="n">
-        <v>261.69</v>
+        <v>231.9</v>
       </c>
       <c r="G41" t="n">
-        <v>39.27</v>
+        <v>36.35</v>
       </c>
       <c r="H41" t="n">
-        <v>119.19</v>
+        <v>114.57</v>
       </c>
       <c r="I41" t="n">
         <v>54</v>
       </c>
       <c r="J41" t="n">
-        <v>7.24</v>
+        <v>5.18</v>
       </c>
       <c r="K41" t="n">
-        <v>143.25</v>
+        <v>141.22</v>
       </c>
       <c r="L41" t="n">
-        <v>199.26</v>
+        <v>187.45</v>
       </c>
       <c r="M41" t="n">
-        <v>18.5</v>
+        <v>17.07</v>
       </c>
       <c r="N41" t="n">
-        <v>70.67</v>
+        <v>69.58</v>
       </c>
       <c r="O41" t="n">
-        <v>17.5</v>
+        <v>15.96</v>
       </c>
       <c r="P41" t="n">
-        <v>566.8099999999999</v>
+        <v>567.55</v>
       </c>
       <c r="Q41" t="n">
-        <v>178.08</v>
+        <v>183.28</v>
       </c>
       <c r="R41" t="n">
-        <v>149.54</v>
+        <v>135.97</v>
       </c>
       <c r="S41" t="n">
-        <v>455.34</v>
+        <v>392.81</v>
       </c>
       <c r="T41" t="n">
-        <v>39.17</v>
+        <v>36.99</v>
       </c>
       <c r="U41" t="n">
-        <v>208.49</v>
+        <v>205.81</v>
       </c>
       <c r="V41" t="n">
-        <v>114.45</v>
+        <v>115.43</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45444</v>
+        <v>45413</v>
       </c>
       <c r="B42" t="n">
-        <v>17732.6</v>
+        <v>16735.02</v>
       </c>
       <c r="C42" t="n">
-        <v>210.15</v>
+        <v>191.56</v>
       </c>
       <c r="D42" t="n">
-        <v>189.7</v>
+        <v>191.03</v>
       </c>
       <c r="E42" t="n">
-        <v>193.25</v>
+        <v>176.44</v>
       </c>
       <c r="F42" t="n">
-        <v>253.2</v>
+        <v>261.69</v>
       </c>
       <c r="G42" t="n">
-        <v>39.06</v>
+        <v>39.27</v>
       </c>
       <c r="H42" t="n">
-        <v>122.45</v>
+        <v>119.19</v>
       </c>
       <c r="I42" t="n">
-        <v>57.24</v>
+        <v>54</v>
       </c>
       <c r="J42" t="n">
-        <v>5.16</v>
+        <v>7.24</v>
       </c>
       <c r="K42" t="n">
-        <v>143.9</v>
+        <v>143.25</v>
       </c>
       <c r="L42" t="n">
-        <v>198.89</v>
+        <v>199.26</v>
       </c>
       <c r="M42" t="n">
-        <v>17.42</v>
+        <v>18.5</v>
       </c>
       <c r="N42" t="n">
-        <v>70.75</v>
+        <v>70.67</v>
       </c>
       <c r="O42" t="n">
-        <v>18.36</v>
+        <v>17.5</v>
       </c>
       <c r="P42" t="n">
-        <v>551.86</v>
+        <v>566.8099999999999</v>
       </c>
       <c r="Q42" t="n">
-        <v>197.88</v>
+        <v>178.08</v>
       </c>
       <c r="R42" t="n">
-        <v>172.08</v>
+        <v>149.54</v>
       </c>
       <c r="S42" t="n">
-        <v>468.72</v>
+        <v>455.34</v>
       </c>
       <c r="T42" t="n">
-        <v>39.26</v>
+        <v>39.17</v>
       </c>
       <c r="U42" t="n">
-        <v>211.07</v>
+        <v>208.49</v>
       </c>
       <c r="V42" t="n">
-        <v>113.27</v>
+        <v>114.45</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45474</v>
+        <v>45444</v>
       </c>
       <c r="B43" t="n">
-        <v>17599.4</v>
+        <v>17732.6</v>
       </c>
       <c r="C43" t="n">
-        <v>221.58</v>
+        <v>210.15</v>
       </c>
       <c r="D43" t="n">
-        <v>216.88</v>
+        <v>189.7</v>
       </c>
       <c r="E43" t="n">
-        <v>186.98</v>
+        <v>193.25</v>
       </c>
       <c r="F43" t="n">
-        <v>258.89</v>
+        <v>253.2</v>
       </c>
       <c r="G43" t="n">
-        <v>39.83</v>
+        <v>39.06</v>
       </c>
       <c r="H43" t="n">
-        <v>140.6</v>
+        <v>122.45</v>
       </c>
       <c r="I43" t="n">
-        <v>55.92</v>
+        <v>57.24</v>
       </c>
       <c r="J43" t="n">
-        <v>5.47</v>
+        <v>5.16</v>
       </c>
       <c r="K43" t="n">
-        <v>155.41</v>
+        <v>143.9</v>
       </c>
       <c r="L43" t="n">
-        <v>209.26</v>
+        <v>198.89</v>
       </c>
       <c r="M43" t="n">
-        <v>18.22</v>
+        <v>17.42</v>
       </c>
       <c r="N43" t="n">
-        <v>71.77</v>
+        <v>70.75</v>
       </c>
       <c r="O43" t="n">
-        <v>18.49</v>
+        <v>18.36</v>
       </c>
       <c r="P43" t="n">
-        <v>612.5</v>
+        <v>551.86</v>
       </c>
       <c r="Q43" t="n">
-        <v>232.07</v>
+        <v>197.88</v>
       </c>
       <c r="R43" t="n">
-        <v>164.67</v>
+        <v>172.08</v>
       </c>
       <c r="S43" t="n">
-        <v>495.72</v>
+        <v>468.72</v>
       </c>
       <c r="T43" t="n">
-        <v>38.57</v>
+        <v>39.26</v>
       </c>
       <c r="U43" t="n">
-        <v>201.25</v>
+        <v>211.07</v>
       </c>
       <c r="V43" t="n">
-        <v>116.68</v>
+        <v>113.27</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45505</v>
+        <v>45474</v>
       </c>
       <c r="B44" t="n">
-        <v>17713.62</v>
+        <v>17599.4</v>
       </c>
       <c r="C44" t="n">
-        <v>228.48</v>
+        <v>221.58</v>
       </c>
       <c r="D44" t="n">
-        <v>220.48</v>
+        <v>216.88</v>
       </c>
       <c r="E44" t="n">
-        <v>178.5</v>
+        <v>186.98</v>
       </c>
       <c r="F44" t="n">
-        <v>275.5</v>
+        <v>258.89</v>
       </c>
       <c r="G44" t="n">
-        <v>40.26</v>
+        <v>39.83</v>
       </c>
       <c r="H44" t="n">
-        <v>141.63</v>
+        <v>140.6</v>
       </c>
       <c r="I44" t="n">
-        <v>55.4</v>
+        <v>55.92</v>
       </c>
       <c r="J44" t="n">
-        <v>5.91</v>
+        <v>5.47</v>
       </c>
       <c r="K44" t="n">
-        <v>163.3</v>
+        <v>155.41</v>
       </c>
       <c r="L44" t="n">
-        <v>222.28</v>
+        <v>209.26</v>
       </c>
       <c r="M44" t="n">
-        <v>19.67</v>
+        <v>18.22</v>
       </c>
       <c r="N44" t="n">
-        <v>70.23999999999999</v>
+        <v>71.77</v>
       </c>
       <c r="O44" t="n">
-        <v>19.4</v>
+        <v>18.49</v>
       </c>
       <c r="P44" t="n">
-        <v>614.22</v>
+        <v>612.5</v>
       </c>
       <c r="Q44" t="n">
-        <v>214.11</v>
+        <v>232.07</v>
       </c>
       <c r="R44" t="n">
-        <v>170.53</v>
+        <v>164.67</v>
       </c>
       <c r="S44" t="n">
-        <v>495.89</v>
+        <v>495.72</v>
       </c>
       <c r="T44" t="n">
-        <v>40.42</v>
+        <v>38.57</v>
       </c>
       <c r="U44" t="n">
-        <v>210.57</v>
+        <v>201.25</v>
       </c>
       <c r="V44" t="n">
-        <v>116.04</v>
+        <v>116.68</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>45536</v>
+        <v>45505</v>
       </c>
       <c r="B45" t="n">
-        <v>18189.17</v>
+        <v>17713.62</v>
       </c>
       <c r="C45" t="n">
-        <v>232.74</v>
+        <v>228.48</v>
       </c>
       <c r="D45" t="n">
-        <v>228.85</v>
+        <v>220.48</v>
       </c>
       <c r="E45" t="n">
-        <v>186.33</v>
+        <v>178.5</v>
       </c>
       <c r="F45" t="n">
-        <v>294.16</v>
+        <v>275.5</v>
       </c>
       <c r="G45" t="n">
-        <v>39.2</v>
+        <v>40.26</v>
       </c>
       <c r="H45" t="n">
-        <v>152.34</v>
+        <v>141.63</v>
       </c>
       <c r="I45" t="n">
-        <v>58.05</v>
+        <v>55.4</v>
       </c>
       <c r="J45" t="n">
-        <v>5.25</v>
+        <v>5.91</v>
       </c>
       <c r="K45" t="n">
-        <v>160.77</v>
+        <v>163.3</v>
       </c>
       <c r="L45" t="n">
-        <v>208.5</v>
+        <v>222.28</v>
       </c>
       <c r="M45" t="n">
-        <v>19.74</v>
+        <v>19.67</v>
       </c>
       <c r="N45" t="n">
-        <v>65.26000000000001</v>
+        <v>70.23999999999999</v>
       </c>
       <c r="O45" t="n">
-        <v>21.45</v>
+        <v>19.4</v>
       </c>
       <c r="P45" t="n">
-        <v>617.72</v>
+        <v>614.22</v>
       </c>
       <c r="Q45" t="n">
-        <v>261.63</v>
+        <v>214.11</v>
       </c>
       <c r="R45" t="n">
-        <v>172.48</v>
+        <v>170.53</v>
       </c>
       <c r="S45" t="n">
-        <v>465.08</v>
+        <v>495.89</v>
       </c>
       <c r="T45" t="n">
-        <v>43.45</v>
+        <v>40.42</v>
       </c>
       <c r="U45" t="n">
-        <v>206.16</v>
+        <v>210.57</v>
       </c>
       <c r="V45" t="n">
-        <v>116.26</v>
+        <v>116.04</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>45566</v>
+        <v>45536</v>
       </c>
       <c r="B46" t="n">
-        <v>18095.15</v>
+        <v>18189.17</v>
       </c>
       <c r="C46" t="n">
-        <v>225.66</v>
+        <v>232.74</v>
       </c>
       <c r="D46" t="n">
-        <v>210.13</v>
+        <v>228.85</v>
       </c>
       <c r="E46" t="n">
-        <v>186.4</v>
+        <v>186.33</v>
       </c>
       <c r="F46" t="n">
-        <v>306.8</v>
+        <v>294.16</v>
       </c>
       <c r="G46" t="n">
-        <v>41.59</v>
+        <v>39.2</v>
       </c>
       <c r="H46" t="n">
-        <v>166.89</v>
+        <v>152.34</v>
       </c>
       <c r="I46" t="n">
-        <v>60.43</v>
+        <v>58.05</v>
       </c>
       <c r="J46" t="n">
-        <v>5.18</v>
+        <v>5.25</v>
       </c>
       <c r="K46" t="n">
-        <v>158.59</v>
+        <v>160.77</v>
       </c>
       <c r="L46" t="n">
-        <v>219.44</v>
+        <v>208.5</v>
       </c>
       <c r="M46" t="n">
-        <v>20.19</v>
+        <v>19.74</v>
       </c>
       <c r="N46" t="n">
-        <v>66.84</v>
+        <v>65.26000000000001</v>
       </c>
       <c r="O46" t="n">
-        <v>21.98</v>
+        <v>21.45</v>
       </c>
       <c r="P46" t="n">
-        <v>545.91</v>
+        <v>617.72</v>
       </c>
       <c r="Q46" t="n">
-        <v>249.85</v>
+        <v>261.63</v>
       </c>
       <c r="R46" t="n">
-        <v>189.94</v>
+        <v>172.48</v>
       </c>
       <c r="S46" t="n">
-        <v>475.98</v>
+        <v>465.08</v>
       </c>
       <c r="T46" t="n">
-        <v>40.76</v>
+        <v>43.45</v>
       </c>
       <c r="U46" t="n">
-        <v>215.13</v>
+        <v>206.16</v>
       </c>
       <c r="V46" t="n">
-        <v>115.83</v>
+        <v>116.26</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>45597</v>
+        <v>45566</v>
       </c>
       <c r="B47" t="n">
-        <v>19218.17</v>
+        <v>18095.15</v>
       </c>
       <c r="C47" t="n">
-        <v>237.07</v>
+        <v>225.66</v>
       </c>
       <c r="D47" t="n">
-        <v>207.16</v>
+        <v>210.13</v>
       </c>
       <c r="E47" t="n">
-        <v>207.89</v>
+        <v>186.4</v>
       </c>
       <c r="F47" t="n">
-        <v>332.29</v>
+        <v>306.8</v>
       </c>
       <c r="G47" t="n">
-        <v>47.25</v>
+        <v>41.59</v>
       </c>
       <c r="H47" t="n">
-        <v>191.09</v>
+        <v>166.89</v>
       </c>
       <c r="I47" t="n">
-        <v>59.79</v>
+        <v>60.43</v>
       </c>
       <c r="J47" t="n">
-        <v>6.33</v>
+        <v>5.18</v>
       </c>
       <c r="K47" t="n">
-        <v>153.78</v>
+        <v>158.59</v>
       </c>
       <c r="L47" t="n">
-        <v>248.44</v>
+        <v>219.44</v>
       </c>
       <c r="M47" t="n">
-        <v>21.6</v>
+        <v>20.19</v>
       </c>
       <c r="N47" t="n">
-        <v>64.06</v>
+        <v>66.84</v>
       </c>
       <c r="O47" t="n">
-        <v>22.87</v>
+        <v>21.98</v>
       </c>
       <c r="P47" t="n">
-        <v>529.24</v>
+        <v>545.91</v>
       </c>
       <c r="Q47" t="n">
-        <v>345.16</v>
+        <v>249.85</v>
       </c>
       <c r="R47" t="n">
-        <v>184.08</v>
+        <v>189.94</v>
       </c>
       <c r="S47" t="n">
-        <v>468.13</v>
+        <v>475.98</v>
       </c>
       <c r="T47" t="n">
-        <v>43.57</v>
+        <v>40.76</v>
       </c>
       <c r="U47" t="n">
-        <v>227.46</v>
+        <v>215.13</v>
       </c>
       <c r="V47" t="n">
-        <v>117</v>
+        <v>115.83</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>45627</v>
+        <v>45597</v>
       </c>
       <c r="B48" t="n">
-        <v>19310.79</v>
+        <v>19218.17</v>
       </c>
       <c r="C48" t="n">
-        <v>250.42</v>
+        <v>237.07</v>
       </c>
       <c r="D48" t="n">
-        <v>181.8</v>
+        <v>207.16</v>
       </c>
       <c r="E48" t="n">
-        <v>219.39</v>
+        <v>207.89</v>
       </c>
       <c r="F48" t="n">
-        <v>288.27</v>
+        <v>332.29</v>
       </c>
       <c r="G48" t="n">
-        <v>43.71</v>
+        <v>47.25</v>
       </c>
       <c r="H48" t="n">
-        <v>172.42</v>
+        <v>191.09</v>
       </c>
       <c r="I48" t="n">
-        <v>60.62</v>
+        <v>59.79</v>
       </c>
       <c r="J48" t="n">
-        <v>7.6</v>
+        <v>6.33</v>
       </c>
       <c r="K48" t="n">
-        <v>144.62</v>
+        <v>153.78</v>
       </c>
       <c r="L48" t="n">
-        <v>238.48</v>
+        <v>248.44</v>
       </c>
       <c r="M48" t="n">
-        <v>20.15</v>
+        <v>21.6</v>
       </c>
       <c r="N48" t="n">
-        <v>62.65</v>
+        <v>64.06</v>
       </c>
       <c r="O48" t="n">
-        <v>22.48</v>
+        <v>22.87</v>
       </c>
       <c r="P48" t="n">
-        <v>519.84</v>
+        <v>529.24</v>
       </c>
       <c r="Q48" t="n">
-        <v>403.84</v>
+        <v>345.16</v>
       </c>
       <c r="R48" t="n">
-        <v>196.86</v>
+        <v>184.08</v>
       </c>
       <c r="S48" t="n">
-        <v>402.7</v>
+        <v>468.13</v>
       </c>
       <c r="T48" t="n">
-        <v>39.29</v>
+        <v>43.57</v>
       </c>
       <c r="U48" t="n">
-        <v>201.11</v>
+        <v>227.46</v>
       </c>
       <c r="V48" t="n">
-        <v>107.57</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
+        <v>45627</v>
+      </c>
+      <c r="B49" t="n">
+        <v>19310.79</v>
+      </c>
+      <c r="C49" t="n">
+        <v>250.42</v>
+      </c>
+      <c r="D49" t="n">
+        <v>181.8</v>
+      </c>
+      <c r="E49" t="n">
+        <v>219.39</v>
+      </c>
+      <c r="F49" t="n">
+        <v>288.27</v>
+      </c>
+      <c r="G49" t="n">
+        <v>43.71</v>
+      </c>
+      <c r="H49" t="n">
+        <v>172.42</v>
+      </c>
+      <c r="I49" t="n">
+        <v>60.62</v>
+      </c>
+      <c r="J49" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="K49" t="n">
+        <v>144.62</v>
+      </c>
+      <c r="L49" t="n">
+        <v>238.48</v>
+      </c>
+      <c r="M49" t="n">
+        <v>20.15</v>
+      </c>
+      <c r="N49" t="n">
+        <v>62.65</v>
+      </c>
+      <c r="O49" t="n">
+        <v>22.48</v>
+      </c>
+      <c r="P49" t="n">
+        <v>519.84</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>403.84</v>
+      </c>
+      <c r="R49" t="n">
+        <v>196.86</v>
+      </c>
+      <c r="S49" t="n">
+        <v>402.7</v>
+      </c>
+      <c r="T49" t="n">
+        <v>39.29</v>
+      </c>
+      <c r="U49" t="n">
+        <v>201.11</v>
+      </c>
+      <c r="V49" t="n">
+        <v>107.57</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="n">
         <v>45658</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B50" t="n">
         <v>19627.44</v>
       </c>
-      <c r="C49" t="n">
+      <c r="C50" t="n">
         <v>236</v>
       </c>
-      <c r="D49" t="n">
+      <c r="D50" t="n">
         <v>184.95</v>
       </c>
-      <c r="E49" t="n">
+      <c r="E50" t="n">
         <v>237.68</v>
       </c>
-      <c r="F49" t="n">
+      <c r="F50" t="n">
         <v>333.21</v>
       </c>
-      <c r="G49" t="n">
+      <c r="G50" t="n">
         <v>46.3</v>
       </c>
-      <c r="H49" t="n">
+      <c r="H50" t="n">
         <v>177.11</v>
       </c>
-      <c r="I49" t="n">
+      <c r="I50" t="n">
         <v>64</v>
       </c>
-      <c r="J49" t="n">
+      <c r="J50" t="n">
         <v>5.85</v>
       </c>
-      <c r="K49" t="n">
+      <c r="K50" t="n">
         <v>152.15</v>
       </c>
-      <c r="L49" t="n">
+      <c r="L50" t="n">
         <v>265.93</v>
       </c>
-      <c r="M49" t="n">
+      <c r="M50" t="n">
         <v>15.65</v>
       </c>
-      <c r="N49" t="n">
+      <c r="N50" t="n">
         <v>65.84999999999999</v>
       </c>
-      <c r="O49" t="n">
+      <c r="O50" t="n">
         <v>23.43</v>
       </c>
-      <c r="P49" t="n">
+      <c r="P50" t="n">
         <v>597.75</v>
       </c>
-      <c r="Q49" t="n">
+      <c r="Q50" t="n">
         <v>404.6</v>
       </c>
-      <c r="R49" t="n">
+      <c r="R50" t="n">
         <v>209.32</v>
       </c>
-      <c r="S49" t="n">
+      <c r="S50" t="n">
         <v>461.68</v>
       </c>
-      <c r="T49" t="n">
+      <c r="T50" t="n">
         <v>38.7</v>
       </c>
-      <c r="U49" t="n">
+      <c r="U50" t="n">
         <v>220.26</v>
       </c>
-      <c r="V49" t="n">
+      <c r="V50" t="n">
         <v>106.83</v>
       </c>
     </row>

</xml_diff>